<commit_message>
Fix: Implemented tracking of Transaction Status
</commit_message>
<xml_diff>
--- a/Data/Temp/TransactionStatus.xlsx
+++ b/Data/Temp/TransactionStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FredrickMutua\Documents\UiPath\FastPipe_Automation\Data\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA8D577-5635-49C0-B2AA-8D5D9F6B17DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEC5624-A290-4247-BE84-DE11802EE5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11835" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -439,7 +439,7 @@
   <dimension ref="A1:AB998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="A1:I1"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1529,7 +1529,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="A1:J1"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1543,7 +1543,8 @@
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="26" width="8.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2598,7 +2599,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Fix: Implemented Outlook notification
</commit_message>
<xml_diff>
--- a/Data/Temp/TransactionStatus.xlsx
+++ b/Data/Temp/TransactionStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FredrickMutua\Documents\UiPath\FastPipe_Automation\Data\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0E8AE2-D96F-4516-857D-550E099DAACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F26086C-3717-4F04-B1FF-0C50ABE11814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Bid Name</t>
   </si>
@@ -47,66 +47,6 @@
   </si>
   <si>
     <t>Date Created/Downloaded</t>
-  </si>
-  <si>
-    <t>Royal Farms 508 Myrtle Beach SC</t>
-  </si>
-  <si>
-    <t>FRONTIER Building Corp.</t>
-  </si>
-  <si>
-    <t>Myrtle Beach</t>
-  </si>
-  <si>
-    <t>SC</t>
-  </si>
-  <si>
-    <t>12/06/2024 11:00 PM</t>
-  </si>
-  <si>
-    <t>C:\Users\FredrickMutua\Documents\UiPath Test Folder\Royal Farms 508 Myrtle Beach SC</t>
-  </si>
-  <si>
-    <t>12/04/2024 09:20:03</t>
-  </si>
-  <si>
-    <t>Starbucks #21264 - Charleston, SC (Savannah HWY) - Renovation</t>
-  </si>
-  <si>
-    <t>Independence Construction</t>
-  </si>
-  <si>
-    <t>Charleston</t>
-  </si>
-  <si>
-    <t>12/06/2024 08:00 PM</t>
-  </si>
-  <si>
-    <t>C:\Users\FredrickMutua\Documents\UiPath Test Folder\Starbucks #21264 - Charleston, SC (Savannah HWY) - Renovation</t>
-  </si>
-  <si>
-    <t>12/04/2024 09:25:39</t>
-  </si>
-  <si>
-    <t>Food Lion #0424 Banner Elk, NC Remodel</t>
-  </si>
-  <si>
-    <t>Newco Construction</t>
-  </si>
-  <si>
-    <t>Banner Elk</t>
-  </si>
-  <si>
-    <t>NC</t>
-  </si>
-  <si>
-    <t>12/07/2024</t>
-  </si>
-  <si>
-    <t>C:\Users\FredrickMutua\Documents\UiPath Test Folder\Food Lion #0424 Banner Elk, NC Remodel Bid Docs</t>
-  </si>
-  <si>
-    <t>12/04/2024 18:38:48</t>
   </si>
 </sst>
 </file>
@@ -484,7 +424,7 @@
   <dimension ref="A1:AB998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -549,84 +489,11 @@
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
     </row>
-    <row r="2" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
+    <row r="2" spans="1:28" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:28">
+      <c r="E3" s="2"/>
     </row>
-    <row r="3" spans="1:28">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
-    </row>
+    <row r="4" spans="1:28" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:28">
       <c r="E5" s="2"/>
     </row>

</xml_diff>

<commit_message>
Fix: Upddated error handling
</commit_message>
<xml_diff>
--- a/Data/Temp/TransactionStatus.xlsx
+++ b/Data/Temp/TransactionStatus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\UiPath\Fast_Pipe_Automation\Data\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD79F4A-DA61-4E88-B6F3-3FE029E87A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF1EEA7-8D52-4A92-9566-DE717771F82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Successful" sheetId="3" r:id="rId1"/>
@@ -112,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="801">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="800">
   <si>
     <t>CITY</t>
   </si>
@@ -2106,9 +2106,6 @@
   </si>
   <si>
     <t>Client Name : Estimating Department Phone Number : (734) 522-3800 Email Address : estimating@ghpastorbids.com</t>
-  </si>
-  <si>
-    <t>Backed Up</t>
   </si>
   <si>
     <r>
@@ -4271,7 +4268,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -5011,11 +5008,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DED64C-ED90-4504-A3DE-AF1F5E294B87}">
   <dimension ref="A1:J290"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" zoomScale="47" zoomScaleNormal="47" workbookViewId="0">
+    <sheetView topLeftCell="A268" zoomScale="47" zoomScaleNormal="47" workbookViewId="0">
       <selection activeCell="F291" sqref="F291"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="20.36328125" style="54" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1796875" style="54" bestFit="1" customWidth="1"/>
@@ -5030,7 +5027,7 @@
     <col min="11" max="16384" width="8.7265625" style="54"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
@@ -5060,7 +5057,7 @@
       </c>
       <c r="J1" s="39"/>
     </row>
-    <row r="2" spans="1:10" ht="18" customHeight="1">
+    <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="65" t="s">
         <v>9</v>
       </c>
@@ -5086,10 +5083,10 @@
         <v>14</v>
       </c>
       <c r="I2" s="51" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="18" customHeight="1">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="65" t="s">
         <v>15</v>
       </c>
@@ -5116,7 +5113,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18" customHeight="1">
+    <row r="4" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="65" t="s">
         <v>20</v>
       </c>
@@ -5143,7 +5140,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="18" customHeight="1">
+    <row r="5" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="65" t="s">
         <v>25</v>
       </c>
@@ -5173,7 +5170,7 @@
       </c>
       <c r="J5" s="51"/>
     </row>
-    <row r="6" spans="1:10" ht="18" customHeight="1">
+    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="65" t="s">
         <v>30</v>
       </c>
@@ -5200,7 +5197,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="18" customHeight="1">
+    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="65" t="s">
         <v>35</v>
       </c>
@@ -5227,7 +5224,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="18" customHeight="1">
+    <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="65" t="s">
         <v>39</v>
       </c>
@@ -5254,7 +5251,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="18" customHeight="1">
+    <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="65" t="s">
         <v>44</v>
       </c>
@@ -5281,7 +5278,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="18" customHeight="1">
+    <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="65" t="s">
         <v>49</v>
       </c>
@@ -5309,7 +5306,7 @@
       </c>
       <c r="J10" s="51"/>
     </row>
-    <row r="11" spans="1:10" ht="18" customHeight="1">
+    <row r="11" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="65" t="s">
         <v>54</v>
       </c>
@@ -5336,7 +5333,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="18" customHeight="1">
+    <row r="12" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="65" t="s">
         <v>58</v>
       </c>
@@ -5360,11 +5357,11 @@
         <v>14</v>
       </c>
       <c r="I12" s="51" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="J12" s="36"/>
     </row>
-    <row r="13" spans="1:10" ht="18" customHeight="1">
+    <row r="13" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="65" t="s">
         <v>60</v>
       </c>
@@ -5391,7 +5388,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="18" customHeight="1">
+    <row r="14" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="65" t="s">
         <v>64</v>
       </c>
@@ -5418,7 +5415,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="18" customHeight="1">
+    <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="65" t="s">
         <v>66</v>
       </c>
@@ -5445,7 +5442,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="18" customHeight="1">
+    <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="65" t="s">
         <v>68</v>
       </c>
@@ -5472,7 +5469,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="18" customHeight="1">
+    <row r="17" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="65" t="s">
         <v>44</v>
       </c>
@@ -5496,10 +5493,10 @@
         <v>14</v>
       </c>
       <c r="I17" s="51" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="18" customHeight="1">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="65" t="s">
         <v>71</v>
       </c>
@@ -5523,10 +5520,10 @@
         <v>14</v>
       </c>
       <c r="I18" s="54" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="18" customHeight="1">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="35" t="s">
         <v>35</v>
       </c>
@@ -5550,10 +5547,10 @@
         <v>14</v>
       </c>
       <c r="I19" s="36" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="18" customHeight="1">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="65" t="s">
         <v>76</v>
       </c>
@@ -5577,10 +5574,10 @@
         <v>14</v>
       </c>
       <c r="I20" s="51" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="18" customHeight="1">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="65" t="s">
         <v>80</v>
       </c>
@@ -5607,7 +5604,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="18" customHeight="1">
+    <row r="22" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="65" t="s">
         <v>82</v>
       </c>
@@ -5631,10 +5628,10 @@
         <v>14</v>
       </c>
       <c r="I22" s="51" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="18" customHeight="1">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="65" t="s">
         <v>85</v>
       </c>
@@ -5658,10 +5655,10 @@
         <v>87</v>
       </c>
       <c r="I23" s="54" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="18" customHeight="1">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="65" t="s">
         <v>88</v>
       </c>
@@ -5685,10 +5682,10 @@
         <v>14</v>
       </c>
       <c r="I24" s="51" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="18" customHeight="1">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="65" t="s">
         <v>92</v>
       </c>
@@ -5712,10 +5709,10 @@
         <v>14</v>
       </c>
       <c r="I25" s="54" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="18" customHeight="1">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="30" t="s">
         <v>94</v>
       </c>
@@ -5741,10 +5738,10 @@
         <v>14</v>
       </c>
       <c r="I26" s="54" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="18" customHeight="1">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="65" t="s">
         <v>97</v>
       </c>
@@ -5768,10 +5765,10 @@
         <v>14</v>
       </c>
       <c r="I27" s="51" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="18" customHeight="1">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="65" t="s">
         <v>99</v>
       </c>
@@ -5795,10 +5792,10 @@
         <v>14</v>
       </c>
       <c r="I28" s="51" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="18" customHeight="1">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="65" t="s">
         <v>102</v>
       </c>
@@ -5822,10 +5819,10 @@
         <v>14</v>
       </c>
       <c r="I29" s="54" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="18" customHeight="1">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="30" t="s">
         <v>105</v>
       </c>
@@ -5849,10 +5846,10 @@
         <v>14</v>
       </c>
       <c r="I30" s="54" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="18" customHeight="1">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="65" t="s">
         <v>108</v>
       </c>
@@ -5876,11 +5873,11 @@
         <v>14</v>
       </c>
       <c r="I31" s="54" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="J31" s="51"/>
     </row>
-    <row r="32" spans="1:10" ht="18" customHeight="1">
+    <row r="32" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="30" t="s">
         <v>112</v>
       </c>
@@ -5906,11 +5903,11 @@
         <v>14</v>
       </c>
       <c r="I32" s="54" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="J32" s="51"/>
     </row>
-    <row r="33" spans="1:10" ht="18" customHeight="1">
+    <row r="33" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="65" t="s">
         <v>112</v>
       </c>
@@ -5936,11 +5933,11 @@
         <v>14</v>
       </c>
       <c r="I33" s="56" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="J33" s="51"/>
     </row>
-    <row r="34" spans="1:10" ht="18" customHeight="1">
+    <row r="34" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="65" t="s">
         <v>118</v>
       </c>
@@ -5968,7 +5965,7 @@
       </c>
       <c r="J34" s="51"/>
     </row>
-    <row r="35" spans="1:10" ht="18" customHeight="1">
+    <row r="35" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="65" t="s">
         <v>122</v>
       </c>
@@ -5998,7 +5995,7 @@
       </c>
       <c r="J35" s="51"/>
     </row>
-    <row r="36" spans="1:10" ht="18" customHeight="1">
+    <row r="36" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="65" t="s">
         <v>127</v>
       </c>
@@ -6022,11 +6019,11 @@
         <v>14</v>
       </c>
       <c r="I36" s="51" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="J36" s="51"/>
     </row>
-    <row r="37" spans="1:10" ht="18" customHeight="1">
+    <row r="37" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="65" t="s">
         <v>130</v>
       </c>
@@ -6050,10 +6047,10 @@
         <v>14</v>
       </c>
       <c r="I37" s="51" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="18" customHeight="1">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="65" t="s">
         <v>133</v>
       </c>
@@ -6077,10 +6074,10 @@
         <v>14</v>
       </c>
       <c r="I38" s="51" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="18" customHeight="1">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="65" t="s">
         <v>135</v>
       </c>
@@ -6104,10 +6101,10 @@
         <v>14</v>
       </c>
       <c r="I39" s="26" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="18" customHeight="1">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="65" t="s">
         <v>138</v>
       </c>
@@ -6131,10 +6128,10 @@
         <v>14</v>
       </c>
       <c r="I40" s="51" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="18" customHeight="1">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="65" t="s">
         <v>141</v>
       </c>
@@ -6158,11 +6155,11 @@
         <v>14</v>
       </c>
       <c r="I41" s="54" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="J41" s="55"/>
     </row>
-    <row r="42" spans="1:10" ht="18" customHeight="1">
+    <row r="42" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="65" t="s">
         <v>144</v>
       </c>
@@ -6192,7 +6189,7 @@
       </c>
       <c r="J42" s="51"/>
     </row>
-    <row r="43" spans="1:10" ht="18" customHeight="1">
+    <row r="43" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="65" t="s">
         <v>149</v>
       </c>
@@ -6218,11 +6215,11 @@
         <v>14</v>
       </c>
       <c r="I43" s="54" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="J43" s="51"/>
     </row>
-    <row r="44" spans="1:10" ht="18" customHeight="1">
+    <row r="44" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="65" t="s">
         <v>152</v>
       </c>
@@ -6248,11 +6245,11 @@
         <v>14</v>
       </c>
       <c r="I44" s="54" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="J44" s="51"/>
     </row>
-    <row r="45" spans="1:10" ht="18" customHeight="1">
+    <row r="45" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="65" t="s">
         <v>156</v>
       </c>
@@ -6278,11 +6275,11 @@
         <v>14</v>
       </c>
       <c r="I45" s="54" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="J45" s="51"/>
     </row>
-    <row r="46" spans="1:10" ht="18" customHeight="1">
+    <row r="46" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="65" t="s">
         <v>160</v>
       </c>
@@ -6308,11 +6305,11 @@
         <v>14</v>
       </c>
       <c r="I46" s="51" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="J46" s="51"/>
     </row>
-    <row r="47" spans="1:10" ht="18" customHeight="1">
+    <row r="47" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="65" t="s">
         <v>164</v>
       </c>
@@ -6338,11 +6335,11 @@
         <v>14</v>
       </c>
       <c r="I47" s="54" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="J47" s="51"/>
     </row>
-    <row r="48" spans="1:10" ht="18" customHeight="1">
+    <row r="48" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="25"/>
       <c r="B48" s="24" t="s">
         <v>16</v>
@@ -6366,11 +6363,11 @@
         <v>14</v>
       </c>
       <c r="I48" s="55" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="J48" s="51"/>
     </row>
-    <row r="49" spans="1:10" ht="20" customHeight="1">
+    <row r="49" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="65" t="s">
         <v>112</v>
       </c>
@@ -6396,11 +6393,11 @@
         <v>14</v>
       </c>
       <c r="I49" s="54" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="J49" s="51"/>
     </row>
-    <row r="50" spans="1:10" ht="40" customHeight="1">
+    <row r="50" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="65" t="s">
         <v>170</v>
       </c>
@@ -6426,11 +6423,11 @@
         <v>14</v>
       </c>
       <c r="I50" s="45" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="J50" s="51"/>
     </row>
-    <row r="51" spans="1:10" ht="20" customHeight="1">
+    <row r="51" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="65" t="s">
         <v>173</v>
       </c>
@@ -6456,11 +6453,11 @@
         <v>14</v>
       </c>
       <c r="I51" s="44" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="J51" s="51"/>
     </row>
-    <row r="52" spans="1:10" ht="21" customHeight="1">
+    <row r="52" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="65" t="s">
         <v>102</v>
       </c>
@@ -6486,11 +6483,11 @@
         <v>14</v>
       </c>
       <c r="I52" s="62" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="J52" s="51"/>
     </row>
-    <row r="53" spans="1:10" ht="21" customHeight="1">
+    <row r="53" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="65" t="s">
         <v>177</v>
       </c>
@@ -6516,11 +6513,11 @@
         <v>14</v>
       </c>
       <c r="I53" s="62" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="J53" s="51"/>
     </row>
-    <row r="54" spans="1:10" ht="20" customHeight="1">
+    <row r="54" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="65" t="s">
         <v>118</v>
       </c>
@@ -6546,11 +6543,11 @@
         <v>14</v>
       </c>
       <c r="I54" s="58" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="J54" s="51"/>
     </row>
-    <row r="55" spans="1:10" ht="20" customHeight="1">
+    <row r="55" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="65" t="s">
         <v>180</v>
       </c>
@@ -6576,11 +6573,11 @@
         <v>14</v>
       </c>
       <c r="I55" s="43" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="J55" s="51"/>
     </row>
-    <row r="56" spans="1:10" ht="20" customHeight="1">
+    <row r="56" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A56" s="65" t="s">
         <v>183</v>
       </c>
@@ -6606,11 +6603,11 @@
         <v>14</v>
       </c>
       <c r="I56" s="56" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="J56" s="51"/>
     </row>
-    <row r="57" spans="1:10" ht="20" customHeight="1">
+    <row r="57" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A57" s="65" t="s">
         <v>185</v>
       </c>
@@ -6636,11 +6633,11 @@
         <v>14</v>
       </c>
       <c r="I57" s="56" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="J57" s="51"/>
     </row>
-    <row r="58" spans="1:10" ht="20" customHeight="1">
+    <row r="58" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" s="65" t="s">
         <v>188</v>
       </c>
@@ -6666,10 +6663,10 @@
         <v>14</v>
       </c>
       <c r="I58" s="56" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="20.5" customHeight="1">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="20.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A59" s="65" t="s">
         <v>190</v>
       </c>
@@ -6695,11 +6692,11 @@
         <v>14</v>
       </c>
       <c r="I59" s="56" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="J59" s="51"/>
     </row>
-    <row r="60" spans="1:10" ht="20" customHeight="1">
+    <row r="60" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A60" s="65" t="s">
         <v>192</v>
       </c>
@@ -6725,11 +6722,11 @@
         <v>14</v>
       </c>
       <c r="I60" s="56" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="J60" s="51"/>
     </row>
-    <row r="61" spans="1:10" ht="20" customHeight="1">
+    <row r="61" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A61" s="65" t="s">
         <v>195</v>
       </c>
@@ -6755,11 +6752,11 @@
         <v>14</v>
       </c>
       <c r="I61" s="56" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="J61" s="51"/>
     </row>
-    <row r="62" spans="1:10" ht="20" customHeight="1">
+    <row r="62" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="65" t="s">
         <v>198</v>
       </c>
@@ -6787,7 +6784,7 @@
       <c r="I62" s="44"/>
       <c r="J62" s="51"/>
     </row>
-    <row r="63" spans="1:10" ht="20.5" customHeight="1">
+    <row r="63" spans="1:10" ht="20.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A63" s="65" t="s">
         <v>201</v>
       </c>
@@ -6813,11 +6810,11 @@
         <v>14</v>
       </c>
       <c r="I63" s="56" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="J63" s="51"/>
     </row>
-    <row r="64" spans="1:10" ht="20" customHeight="1">
+    <row r="64" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A64" s="65" t="s">
         <v>204</v>
       </c>
@@ -6843,11 +6840,11 @@
         <v>14</v>
       </c>
       <c r="I64" s="51" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="J64" s="51"/>
     </row>
-    <row r="65" spans="1:10" ht="40" customHeight="1">
+    <row r="65" spans="1:10" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="30" t="s">
         <v>208</v>
       </c>
@@ -6873,11 +6870,11 @@
         <v>14</v>
       </c>
       <c r="I65" s="42" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="J65" s="51"/>
     </row>
-    <row r="66" spans="1:10" ht="20" customHeight="1">
+    <row r="66" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="65" t="s">
         <v>170</v>
       </c>
@@ -6907,7 +6904,7 @@
       </c>
       <c r="J66" s="51"/>
     </row>
-    <row r="67" spans="1:10" ht="41" customHeight="1">
+    <row r="67" spans="1:10" ht="41" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A67" s="65" t="s">
         <v>211</v>
       </c>
@@ -6933,11 +6930,11 @@
         <v>14</v>
       </c>
       <c r="I67" s="41" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="J67" s="51"/>
     </row>
-    <row r="68" spans="1:10" ht="20.5" customHeight="1">
+    <row r="68" spans="1:10" ht="20.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A68" s="65" t="s">
         <v>214</v>
       </c>
@@ -6963,10 +6960,10 @@
         <v>14</v>
       </c>
       <c r="I68" s="56" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="20" customHeight="1">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A69" s="30" t="s">
         <v>216</v>
       </c>
@@ -6992,11 +6989,11 @@
         <v>14</v>
       </c>
       <c r="I69" s="54" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="J69" s="51"/>
     </row>
-    <row r="70" spans="1:10" ht="20" customHeight="1">
+    <row r="70" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A70" s="30" t="s">
         <v>170</v>
       </c>
@@ -7022,11 +7019,11 @@
         <v>14</v>
       </c>
       <c r="I70" s="56" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="J70" s="51"/>
     </row>
-    <row r="71" spans="1:10" ht="20.5" customHeight="1">
+    <row r="71" spans="1:10" ht="20.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A71" s="65" t="s">
         <v>188</v>
       </c>
@@ -7052,11 +7049,11 @@
         <v>14</v>
       </c>
       <c r="I71" s="56" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="J71" s="51"/>
     </row>
-    <row r="72" spans="1:10" ht="18" customHeight="1">
+    <row r="72" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="65" t="s">
         <v>219</v>
       </c>
@@ -7082,11 +7079,11 @@
         <v>14</v>
       </c>
       <c r="I72" s="51" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="J72" s="51"/>
     </row>
-    <row r="73" spans="1:10" ht="18" customHeight="1">
+    <row r="73" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="65" t="s">
         <v>219</v>
       </c>
@@ -7112,11 +7109,11 @@
         <v>14</v>
       </c>
       <c r="I73" s="51" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="J73" s="51"/>
     </row>
-    <row r="74" spans="1:10" ht="18" customHeight="1">
+    <row r="74" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A74" s="65" t="s">
         <v>223</v>
       </c>
@@ -7142,11 +7139,11 @@
         <v>14</v>
       </c>
       <c r="I74" s="52" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="J74" s="51"/>
     </row>
-    <row r="75" spans="1:10" ht="18" customHeight="1">
+    <row r="75" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="65" t="s">
         <v>225</v>
       </c>
@@ -7176,7 +7173,7 @@
       </c>
       <c r="J75" s="51"/>
     </row>
-    <row r="76" spans="1:10" ht="18" customHeight="1">
+    <row r="76" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="65" t="s">
         <v>180</v>
       </c>
@@ -7202,11 +7199,11 @@
         <v>14</v>
       </c>
       <c r="I76" s="77" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="J76" s="51"/>
     </row>
-    <row r="77" spans="1:10" ht="36" customHeight="1">
+    <row r="77" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="65" t="s">
         <v>44</v>
       </c>
@@ -7232,11 +7229,11 @@
         <v>14</v>
       </c>
       <c r="I77" s="77" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="J77" s="51"/>
     </row>
-    <row r="78" spans="1:10" ht="18" customHeight="1">
+    <row r="78" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="65" t="s">
         <v>170</v>
       </c>
@@ -7266,7 +7263,7 @@
       </c>
       <c r="J78" s="51"/>
     </row>
-    <row r="79" spans="1:10" ht="18" customHeight="1">
+    <row r="79" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A79" s="65" t="s">
         <v>233</v>
       </c>
@@ -7292,11 +7289,11 @@
         <v>14</v>
       </c>
       <c r="I79" s="54" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="J79" s="51"/>
     </row>
-    <row r="80" spans="1:10" ht="18" customHeight="1">
+    <row r="80" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A80" s="65" t="s">
         <v>118</v>
       </c>
@@ -7322,11 +7319,11 @@
         <v>14</v>
       </c>
       <c r="I80" s="59" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="J80" s="51"/>
     </row>
-    <row r="81" spans="1:10" ht="18" customHeight="1">
+    <row r="81" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="65" t="s">
         <v>112</v>
       </c>
@@ -7351,7 +7348,7 @@
       </c>
       <c r="J81" s="51"/>
     </row>
-    <row r="82" spans="1:10" ht="18" customHeight="1">
+    <row r="82" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="65" t="s">
         <v>237</v>
       </c>
@@ -7381,7 +7378,7 @@
       </c>
       <c r="J82" s="51"/>
     </row>
-    <row r="83" spans="1:10" ht="18" customHeight="1">
+    <row r="83" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="65" t="s">
         <v>241</v>
       </c>
@@ -7411,7 +7408,7 @@
       </c>
       <c r="J83" s="51"/>
     </row>
-    <row r="84" spans="1:10" ht="18" customHeight="1">
+    <row r="84" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A84" s="65" t="s">
         <v>223</v>
       </c>
@@ -7437,11 +7434,11 @@
         <v>14</v>
       </c>
       <c r="I84" s="54" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="J84" s="51"/>
     </row>
-    <row r="85" spans="1:10" ht="18" customHeight="1">
+    <row r="85" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A85" s="65" t="s">
         <v>245</v>
       </c>
@@ -7467,11 +7464,11 @@
         <v>14</v>
       </c>
       <c r="I85" s="54" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="J85" s="51"/>
     </row>
-    <row r="86" spans="1:10" ht="36" customHeight="1">
+    <row r="86" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A86" s="65" t="s">
         <v>248</v>
       </c>
@@ -7497,11 +7494,11 @@
         <v>14</v>
       </c>
       <c r="I86" s="59" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="J86" s="51"/>
     </row>
-    <row r="87" spans="1:10" ht="18" customHeight="1">
+    <row r="87" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A87" s="65" t="s">
         <v>250</v>
       </c>
@@ -7527,11 +7524,11 @@
         <v>14</v>
       </c>
       <c r="I87" s="56" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="J87" s="51"/>
     </row>
-    <row r="88" spans="1:10" ht="18" customHeight="1">
+    <row r="88" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="65" t="s">
         <v>253</v>
       </c>
@@ -7557,11 +7554,11 @@
         <v>14</v>
       </c>
       <c r="I88" s="56" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J88" s="51"/>
     </row>
-    <row r="89" spans="1:10" ht="18" customHeight="1">
+    <row r="89" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="65" t="s">
         <v>256</v>
       </c>
@@ -7591,7 +7588,7 @@
       </c>
       <c r="J89" s="51"/>
     </row>
-    <row r="90" spans="1:10" ht="35" customHeight="1">
+    <row r="90" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="65" t="s">
         <v>256</v>
       </c>
@@ -7621,7 +7618,7 @@
       </c>
       <c r="J90" s="51"/>
     </row>
-    <row r="91" spans="1:10" ht="18" customHeight="1">
+    <row r="91" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A91" s="65" t="s">
         <v>44</v>
       </c>
@@ -7647,11 +7644,11 @@
         <v>14</v>
       </c>
       <c r="I91" s="57" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="J91" s="51"/>
     </row>
-    <row r="92" spans="1:10" ht="20" customHeight="1">
+    <row r="92" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A92" s="65" t="s">
         <v>44</v>
       </c>
@@ -7677,11 +7674,11 @@
         <v>14</v>
       </c>
       <c r="I92" s="51" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="J92" s="51"/>
     </row>
-    <row r="93" spans="1:10" ht="18" customHeight="1">
+    <row r="93" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A93" s="65" t="s">
         <v>253</v>
       </c>
@@ -7705,11 +7702,11 @@
       </c>
       <c r="H93" s="69"/>
       <c r="I93" s="57" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="J93" s="51"/>
     </row>
-    <row r="94" spans="1:10" ht="18" customHeight="1">
+    <row r="94" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A94" s="65" t="s">
         <v>263</v>
       </c>
@@ -7735,11 +7732,11 @@
         <v>14</v>
       </c>
       <c r="I94" s="54" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="J94" s="51"/>
     </row>
-    <row r="95" spans="1:10" ht="35" customHeight="1">
+    <row r="95" spans="1:10" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="65" t="s">
         <v>265</v>
       </c>
@@ -7765,11 +7762,11 @@
         <v>14</v>
       </c>
       <c r="I95" s="52" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="J95" s="51"/>
     </row>
-    <row r="96" spans="1:10" ht="18" customHeight="1">
+    <row r="96" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="65" t="s">
         <v>267</v>
       </c>
@@ -7799,7 +7796,7 @@
       </c>
       <c r="J96" s="51"/>
     </row>
-    <row r="97" spans="1:10" ht="20" customHeight="1">
+    <row r="97" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A97" s="65" t="s">
         <v>270</v>
       </c>
@@ -7825,11 +7822,11 @@
         <v>14</v>
       </c>
       <c r="I97" s="56" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="J97" s="51"/>
     </row>
-    <row r="98" spans="1:10" ht="18" customHeight="1">
+    <row r="98" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A98" s="65" t="s">
         <v>272</v>
       </c>
@@ -7855,11 +7852,11 @@
         <v>14</v>
       </c>
       <c r="I98" s="51" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="J98" s="51"/>
     </row>
-    <row r="99" spans="1:10" ht="18" customHeight="1">
+    <row r="99" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A99" s="65" t="s">
         <v>274</v>
       </c>
@@ -7885,11 +7882,11 @@
         <v>14</v>
       </c>
       <c r="I99" s="52" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="J99" s="51"/>
     </row>
-    <row r="100" spans="1:10" ht="18" customHeight="1">
+    <row r="100" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A100" s="65" t="s">
         <v>276</v>
       </c>
@@ -7915,11 +7912,11 @@
         <v>14</v>
       </c>
       <c r="I100" s="56" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="J100" s="51"/>
     </row>
-    <row r="101" spans="1:10" ht="18" customHeight="1">
+    <row r="101" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A101" s="65" t="s">
         <v>277</v>
       </c>
@@ -7945,11 +7942,11 @@
         <v>14</v>
       </c>
       <c r="I101" s="59" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="J101" s="51"/>
     </row>
-    <row r="102" spans="1:10" ht="18" customHeight="1">
+    <row r="102" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="65" t="s">
         <v>279</v>
       </c>
@@ -7975,11 +7972,11 @@
         <v>14</v>
       </c>
       <c r="I102" s="56" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="J102" s="51"/>
     </row>
-    <row r="103" spans="1:10" ht="18" customHeight="1">
+    <row r="103" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A103" s="65" t="s">
         <v>272</v>
       </c>
@@ -8005,11 +8002,11 @@
         <v>14</v>
       </c>
       <c r="I103" s="56" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="J103" s="51"/>
     </row>
-    <row r="104" spans="1:10" ht="18" customHeight="1">
+    <row r="104" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A104" s="65" t="s">
         <v>118</v>
       </c>
@@ -8035,11 +8032,11 @@
         <v>14</v>
       </c>
       <c r="I104" s="56" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="J104" s="51"/>
     </row>
-    <row r="105" spans="1:10" ht="18" customHeight="1">
+    <row r="105" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="65" t="s">
         <v>285</v>
       </c>
@@ -8068,7 +8065,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="18" customHeight="1">
+    <row r="106" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="65" t="s">
         <v>288</v>
       </c>
@@ -8097,7 +8094,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="18.5" customHeight="1">
+    <row r="107" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A107" s="30" t="s">
         <v>289</v>
       </c>
@@ -8123,10 +8120,10 @@
         <v>14</v>
       </c>
       <c r="I107" s="54" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" ht="18.5" customHeight="1">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A108" s="65" t="s">
         <v>214</v>
       </c>
@@ -8152,10 +8149,10 @@
         <v>14</v>
       </c>
       <c r="I108" s="54" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" ht="20" customHeight="1">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A109" s="65" t="s">
         <v>291</v>
       </c>
@@ -8181,11 +8178,11 @@
         <v>14</v>
       </c>
       <c r="I109" s="51" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="J109" s="51"/>
     </row>
-    <row r="110" spans="1:10" ht="18" customHeight="1">
+    <row r="110" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="30" t="s">
         <v>160</v>
       </c>
@@ -8215,7 +8212,7 @@
       </c>
       <c r="J110" s="51"/>
     </row>
-    <row r="111" spans="1:10" ht="18" customHeight="1">
+    <row r="111" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="65" t="s">
         <v>295</v>
       </c>
@@ -8241,11 +8238,11 @@
         <v>14</v>
       </c>
       <c r="I111" s="58" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="J111" s="51"/>
     </row>
-    <row r="112" spans="1:10" ht="18" customHeight="1">
+    <row r="112" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A112" s="65" t="s">
         <v>297</v>
       </c>
@@ -8271,11 +8268,11 @@
         <v>14</v>
       </c>
       <c r="I112" s="54" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="J112" s="51"/>
     </row>
-    <row r="113" spans="1:10" ht="18" customHeight="1">
+    <row r="113" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="65" t="s">
         <v>300</v>
       </c>
@@ -8301,11 +8298,11 @@
         <v>14</v>
       </c>
       <c r="I113" s="30" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="J113" s="51"/>
     </row>
-    <row r="114" spans="1:10" ht="18" customHeight="1">
+    <row r="114" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A114" s="30" t="s">
         <v>302</v>
       </c>
@@ -8331,11 +8328,11 @@
         <v>14</v>
       </c>
       <c r="I114" s="59" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="J114" s="51"/>
     </row>
-    <row r="115" spans="1:10" ht="18" customHeight="1">
+    <row r="115" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A115" s="65" t="s">
         <v>305</v>
       </c>
@@ -8361,11 +8358,11 @@
         <v>14</v>
       </c>
       <c r="I115" s="54" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="J115" s="51"/>
     </row>
-    <row r="116" spans="1:10" ht="18" customHeight="1">
+    <row r="116" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A116" s="65" t="s">
         <v>307</v>
       </c>
@@ -8391,11 +8388,11 @@
         <v>14</v>
       </c>
       <c r="I116" s="54" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="J116" s="51"/>
     </row>
-    <row r="117" spans="1:10" ht="18" customHeight="1">
+    <row r="117" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="30" t="s">
         <v>302</v>
       </c>
@@ -8421,11 +8418,11 @@
         <v>14</v>
       </c>
       <c r="I117" s="59" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="J117" s="51"/>
     </row>
-    <row r="118" spans="1:10" ht="18" customHeight="1">
+    <row r="118" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A118" s="65" t="s">
         <v>118</v>
       </c>
@@ -8451,11 +8448,11 @@
         <v>14</v>
       </c>
       <c r="I118" s="54" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="J118" s="51"/>
     </row>
-    <row r="119" spans="1:10" ht="18" customHeight="1">
+    <row r="119" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A119" s="65" t="s">
         <v>201</v>
       </c>
@@ -8481,11 +8478,11 @@
         <v>14</v>
       </c>
       <c r="I119" s="54" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="J119" s="51"/>
     </row>
-    <row r="120" spans="1:10" ht="18" customHeight="1">
+    <row r="120" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="65" t="s">
         <v>311</v>
       </c>
@@ -8515,7 +8512,7 @@
       </c>
       <c r="J120" s="51"/>
     </row>
-    <row r="121" spans="1:10" ht="18" customHeight="1">
+    <row r="121" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="65" t="s">
         <v>314</v>
       </c>
@@ -8542,7 +8539,7 @@
       </c>
       <c r="J121" s="51"/>
     </row>
-    <row r="122" spans="1:10" ht="18" customHeight="1">
+    <row r="122" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="65" t="s">
         <v>315</v>
       </c>
@@ -8572,7 +8569,7 @@
       </c>
       <c r="J122" s="51"/>
     </row>
-    <row r="123" spans="1:10" ht="18" customHeight="1">
+    <row r="123" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="65" t="s">
         <v>318</v>
       </c>
@@ -8598,11 +8595,11 @@
         <v>14</v>
       </c>
       <c r="I123" s="51" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="J123" s="51"/>
     </row>
-    <row r="124" spans="1:10" ht="18" customHeight="1">
+    <row r="124" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" s="65" t="s">
         <v>320</v>
       </c>
@@ -8628,11 +8625,11 @@
         <v>14</v>
       </c>
       <c r="I124" s="51" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="J124" s="51"/>
     </row>
-    <row r="125" spans="1:10" ht="18" customHeight="1">
+    <row r="125" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="65" t="s">
         <v>112</v>
       </c>
@@ -8662,7 +8659,7 @@
       </c>
       <c r="J125" s="51"/>
     </row>
-    <row r="126" spans="1:10" ht="18" customHeight="1">
+    <row r="126" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="65" t="s">
         <v>323</v>
       </c>
@@ -8688,11 +8685,11 @@
         <v>14</v>
       </c>
       <c r="I126" s="56" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="J126" s="51"/>
     </row>
-    <row r="127" spans="1:10" ht="18" customHeight="1">
+    <row r="127" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="30" t="s">
         <v>216</v>
       </c>
@@ -8722,7 +8719,7 @@
       </c>
       <c r="J127" s="51"/>
     </row>
-    <row r="128" spans="1:10" ht="18" customHeight="1">
+    <row r="128" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A128" s="30" t="s">
         <v>216</v>
       </c>
@@ -8748,11 +8745,11 @@
         <v>14</v>
       </c>
       <c r="I128" s="51" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="J128" s="51"/>
     </row>
-    <row r="129" spans="1:10" ht="18" customHeight="1">
+    <row r="129" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="65" t="s">
         <v>320</v>
       </c>
@@ -8782,7 +8779,7 @@
       </c>
       <c r="J129" s="51"/>
     </row>
-    <row r="130" spans="1:10" ht="18" customHeight="1">
+    <row r="130" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A130" s="65" t="s">
         <v>327</v>
       </c>
@@ -8808,11 +8805,11 @@
         <v>14</v>
       </c>
       <c r="I130" s="56" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="J130" s="51"/>
     </row>
-    <row r="131" spans="1:10" ht="18" customHeight="1">
+    <row r="131" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="65" t="s">
         <v>329</v>
       </c>
@@ -8838,11 +8835,11 @@
         <v>14</v>
       </c>
       <c r="I131" s="54" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="J131" s="51"/>
     </row>
-    <row r="132" spans="1:10" ht="18" customHeight="1">
+    <row r="132" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="65" t="s">
         <v>327</v>
       </c>
@@ -8868,11 +8865,11 @@
         <v>14</v>
       </c>
       <c r="I132" s="56" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="J132" s="51"/>
     </row>
-    <row r="133" spans="1:10" ht="18" customHeight="1">
+    <row r="133" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A133" s="65" t="s">
         <v>330</v>
       </c>
@@ -8898,11 +8895,11 @@
         <v>14</v>
       </c>
       <c r="I133" s="54" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="J133" s="51"/>
     </row>
-    <row r="134" spans="1:10" ht="18" customHeight="1">
+    <row r="134" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A134" s="65" t="s">
         <v>333</v>
       </c>
@@ -8928,11 +8925,11 @@
         <v>14</v>
       </c>
       <c r="I134" s="52" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="J134" s="51"/>
     </row>
-    <row r="135" spans="1:10" ht="18" customHeight="1">
+    <row r="135" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A135" s="65" t="s">
         <v>323</v>
       </c>
@@ -8958,11 +8955,11 @@
         <v>14</v>
       </c>
       <c r="I135" s="56" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="J135" s="51"/>
     </row>
-    <row r="136" spans="1:10" ht="18" customHeight="1">
+    <row r="136" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" s="65" t="s">
         <v>329</v>
       </c>
@@ -8992,7 +8989,7 @@
       </c>
       <c r="J136" s="51"/>
     </row>
-    <row r="137" spans="1:10" ht="18" customHeight="1">
+    <row r="137" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="65" t="s">
         <v>337</v>
       </c>
@@ -9022,7 +9019,7 @@
       </c>
       <c r="J137" s="51"/>
     </row>
-    <row r="138" spans="1:10" ht="18" customHeight="1">
+    <row r="138" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="65" t="s">
         <v>341</v>
       </c>
@@ -9052,7 +9049,7 @@
       </c>
       <c r="J138" s="51"/>
     </row>
-    <row r="139" spans="1:10" ht="20" customHeight="1">
+    <row r="139" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A139" s="65" t="s">
         <v>344</v>
       </c>
@@ -9078,11 +9075,11 @@
         <v>14</v>
       </c>
       <c r="I139" s="54" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="J139" s="51"/>
     </row>
-    <row r="140" spans="1:10" ht="18" customHeight="1">
+    <row r="140" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="65" t="s">
         <v>347</v>
       </c>
@@ -9112,7 +9109,7 @@
       </c>
       <c r="J140" s="51"/>
     </row>
-    <row r="141" spans="1:10" ht="18" customHeight="1">
+    <row r="141" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A141" s="65" t="s">
         <v>350</v>
       </c>
@@ -9138,11 +9135,11 @@
         <v>14</v>
       </c>
       <c r="I141" s="59" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="J141" s="51"/>
     </row>
-    <row r="142" spans="1:10" ht="18" customHeight="1">
+    <row r="142" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" s="65" t="s">
         <v>351</v>
       </c>
@@ -9171,7 +9168,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="18" customHeight="1">
+    <row r="143" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A143" s="65" t="s">
         <v>225</v>
       </c>
@@ -9197,11 +9194,11 @@
         <v>14</v>
       </c>
       <c r="I143" s="54" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="J143" s="51"/>
     </row>
-    <row r="144" spans="1:10" ht="18" customHeight="1">
+    <row r="144" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A144" s="65" t="s">
         <v>54</v>
       </c>
@@ -9227,11 +9224,11 @@
         <v>14</v>
       </c>
       <c r="I144" s="54" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="J144" s="51"/>
     </row>
-    <row r="145" spans="1:10" ht="18" customHeight="1">
+    <row r="145" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A145" s="65" t="s">
         <v>356</v>
       </c>
@@ -9257,11 +9254,11 @@
         <v>14</v>
       </c>
       <c r="I145" s="54" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="J145" s="51"/>
     </row>
-    <row r="146" spans="1:10" ht="18" customHeight="1">
+    <row r="146" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A146" s="30" t="s">
         <v>358</v>
       </c>
@@ -9287,10 +9284,10 @@
         <v>14</v>
       </c>
       <c r="I146" s="62" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="147" spans="1:10" ht="18" customHeight="1">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" s="65" t="s">
         <v>180</v>
       </c>
@@ -9318,7 +9315,7 @@
       <c r="I147" s="51"/>
       <c r="J147" s="51"/>
     </row>
-    <row r="148" spans="1:10" ht="18" customHeight="1">
+    <row r="148" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" s="65" t="s">
         <v>180</v>
       </c>
@@ -9346,7 +9343,7 @@
       <c r="I148" s="51"/>
       <c r="J148" s="51"/>
     </row>
-    <row r="149" spans="1:10" ht="18" customHeight="1">
+    <row r="149" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" s="65" t="s">
         <v>329</v>
       </c>
@@ -9376,7 +9373,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="150" spans="1:10" ht="18" customHeight="1">
+    <row r="150" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" s="65" t="s">
         <v>364</v>
       </c>
@@ -9404,7 +9401,7 @@
       <c r="I150" s="51"/>
       <c r="J150" s="51"/>
     </row>
-    <row r="151" spans="1:10" ht="20" customHeight="1">
+    <row r="151" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A151" s="65" t="s">
         <v>367</v>
       </c>
@@ -9430,10 +9427,10 @@
         <v>14</v>
       </c>
       <c r="I151" s="51" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="152" spans="1:10" ht="18" customHeight="1">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" s="30" t="s">
         <v>370</v>
       </c>
@@ -9462,7 +9459,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="153" spans="1:10" ht="18" customHeight="1">
+    <row r="153" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A153" s="30" t="s">
         <v>373</v>
       </c>
@@ -9488,11 +9485,11 @@
         <v>14</v>
       </c>
       <c r="I153" s="54" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="J153" s="50"/>
     </row>
-    <row r="154" spans="1:10" ht="18" customHeight="1">
+    <row r="154" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A154" s="66" t="s">
         <v>377</v>
       </c>
@@ -9518,11 +9515,11 @@
         <v>14</v>
       </c>
       <c r="I154" s="53" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="J154" s="50"/>
     </row>
-    <row r="155" spans="1:10" ht="18" customHeight="1">
+    <row r="155" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A155" s="66" t="s">
         <v>377</v>
       </c>
@@ -9548,11 +9545,11 @@
         <v>14</v>
       </c>
       <c r="I155" s="50" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="J155" s="50"/>
     </row>
-    <row r="156" spans="1:10" ht="18" customHeight="1">
+    <row r="156" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" s="66" t="s">
         <v>381</v>
       </c>
@@ -9582,7 +9579,7 @@
       </c>
       <c r="J156" s="50"/>
     </row>
-    <row r="157" spans="1:10" ht="18" customHeight="1">
+    <row r="157" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A157" s="66" t="s">
         <v>385</v>
       </c>
@@ -9608,11 +9605,11 @@
         <v>14</v>
       </c>
       <c r="I157" s="50" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="J157" s="50"/>
     </row>
-    <row r="158" spans="1:10" ht="18" customHeight="1">
+    <row r="158" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A158" s="66" t="s">
         <v>54</v>
       </c>
@@ -9638,11 +9635,11 @@
         <v>14</v>
       </c>
       <c r="I158" s="50" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="J158" s="50"/>
     </row>
-    <row r="159" spans="1:10" ht="18" customHeight="1">
+    <row r="159" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="30" t="s">
         <v>389</v>
       </c>
@@ -9671,7 +9668,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="18" customHeight="1">
+    <row r="160" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A160" s="66" t="s">
         <v>118</v>
       </c>
@@ -9697,11 +9694,11 @@
         <v>14</v>
       </c>
       <c r="I160" s="54" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="J160" s="50"/>
     </row>
-    <row r="161" spans="1:10" ht="18" customHeight="1">
+    <row r="161" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A161" s="66" t="s">
         <v>118</v>
       </c>
@@ -9727,11 +9724,11 @@
         <v>14</v>
       </c>
       <c r="I161" s="54" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="J161" s="50"/>
     </row>
-    <row r="162" spans="1:10" ht="18" customHeight="1">
+    <row r="162" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="30" t="s">
         <v>394</v>
       </c>
@@ -9760,7 +9757,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="163" spans="1:10" ht="18" customHeight="1">
+    <row r="163" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A163" s="66" t="s">
         <v>397</v>
       </c>
@@ -9786,11 +9783,11 @@
         <v>14</v>
       </c>
       <c r="I163" s="50" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="J163" s="51"/>
     </row>
-    <row r="164" spans="1:10" ht="18" customHeight="1">
+    <row r="164" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A164" s="66" t="s">
         <v>400</v>
       </c>
@@ -9816,11 +9813,11 @@
         <v>14</v>
       </c>
       <c r="I164" s="50" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="J164" s="51"/>
     </row>
-    <row r="165" spans="1:10" ht="18" customHeight="1">
+    <row r="165" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" s="66" t="s">
         <v>402</v>
       </c>
@@ -9850,7 +9847,7 @@
       </c>
       <c r="J165" s="51"/>
     </row>
-    <row r="166" spans="1:10" ht="18" customHeight="1">
+    <row r="166" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A166" s="65" t="s">
         <v>404</v>
       </c>
@@ -9876,11 +9873,11 @@
         <v>14</v>
       </c>
       <c r="I166" s="52" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="J166" s="51"/>
     </row>
-    <row r="167" spans="1:10" ht="18" customHeight="1">
+    <row r="167" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A167" s="65" t="s">
         <v>406</v>
       </c>
@@ -9906,11 +9903,11 @@
         <v>14</v>
       </c>
       <c r="I167" s="51" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="J167" s="51"/>
     </row>
-    <row r="168" spans="1:10" ht="18" customHeight="1">
+    <row r="168" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A168" s="30" t="s">
         <v>408</v>
       </c>
@@ -9936,10 +9933,10 @@
         <v>14</v>
       </c>
       <c r="I168" s="62" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="169" spans="1:10" ht="18" customHeight="1">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A169" s="30" t="s">
         <v>112</v>
       </c>
@@ -9965,10 +9962,10 @@
         <v>14</v>
       </c>
       <c r="I169" s="50" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="170" spans="1:10" ht="18" customHeight="1">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A170" s="30" t="s">
         <v>412</v>
       </c>
@@ -9994,11 +9991,11 @@
         <v>14</v>
       </c>
       <c r="I170" s="54" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="J170" s="51"/>
     </row>
-    <row r="171" spans="1:10" ht="18" customHeight="1">
+    <row r="171" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A171" s="30" t="s">
         <v>412</v>
       </c>
@@ -10024,11 +10021,11 @@
         <v>14</v>
       </c>
       <c r="I171" s="54" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="J171" s="51"/>
     </row>
-    <row r="172" spans="1:10" ht="18" customHeight="1">
+    <row r="172" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A172" s="30" t="s">
         <v>35</v>
       </c>
@@ -10054,11 +10051,11 @@
         <v>14</v>
       </c>
       <c r="I172" s="62" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="J172" s="51"/>
     </row>
-    <row r="173" spans="1:10" ht="18" customHeight="1">
+    <row r="173" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A173" s="30" t="s">
         <v>300</v>
       </c>
@@ -10084,11 +10081,11 @@
         <v>14</v>
       </c>
       <c r="I173" s="54" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="J173" s="51"/>
     </row>
-    <row r="174" spans="1:10" ht="18" customHeight="1">
+    <row r="174" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A174" s="65" t="s">
         <v>418</v>
       </c>
@@ -10114,11 +10111,11 @@
         <v>14</v>
       </c>
       <c r="I174" s="51" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="J174" s="51"/>
     </row>
-    <row r="175" spans="1:10" ht="18" customHeight="1">
+    <row r="175" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A175" s="65" t="s">
         <v>420</v>
       </c>
@@ -10144,11 +10141,11 @@
         <v>14</v>
       </c>
       <c r="I175" s="54" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="J175" s="51"/>
     </row>
-    <row r="176" spans="1:10" ht="18" customHeight="1">
+    <row r="176" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A176" s="65" t="s">
         <v>422</v>
       </c>
@@ -10174,11 +10171,11 @@
         <v>14</v>
       </c>
       <c r="I176" s="50" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="J176" s="51"/>
     </row>
-    <row r="177" spans="1:10" ht="18" customHeight="1">
+    <row r="177" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A177" s="65" t="s">
         <v>424</v>
       </c>
@@ -10204,11 +10201,11 @@
         <v>14</v>
       </c>
       <c r="I177" s="54" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="J177" s="51"/>
     </row>
-    <row r="178" spans="1:10" ht="20" customHeight="1">
+    <row r="178" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A178" s="65" t="s">
         <v>297</v>
       </c>
@@ -10234,11 +10231,11 @@
         <v>14</v>
       </c>
       <c r="I178" s="56" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="J178" s="51"/>
     </row>
-    <row r="179" spans="1:10" ht="18" customHeight="1">
+    <row r="179" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" s="66" t="s">
         <v>404</v>
       </c>
@@ -10268,7 +10265,7 @@
       </c>
       <c r="J179" s="51"/>
     </row>
-    <row r="180" spans="1:10" ht="18" customHeight="1">
+    <row r="180" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A180" s="30" t="s">
         <v>430</v>
       </c>
@@ -10294,10 +10291,10 @@
         <v>14</v>
       </c>
       <c r="I180" s="54" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="181" spans="1:10" ht="18" customHeight="1">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A181" s="65" t="s">
         <v>344</v>
       </c>
@@ -10323,10 +10320,10 @@
         <v>14</v>
       </c>
       <c r="I181" s="50" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="182" spans="1:10" ht="18" customHeight="1">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" s="65" t="s">
         <v>223</v>
       </c>
@@ -10356,7 +10353,7 @@
       </c>
       <c r="J182" s="51"/>
     </row>
-    <row r="183" spans="1:10" ht="18" customHeight="1">
+    <row r="183" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A183" s="65" t="s">
         <v>9</v>
       </c>
@@ -10382,11 +10379,11 @@
         <v>14</v>
       </c>
       <c r="I183" s="51" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="J183" s="51"/>
     </row>
-    <row r="184" spans="1:10" ht="18" customHeight="1">
+    <row r="184" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A184" s="13" t="s">
         <v>436</v>
       </c>
@@ -10412,11 +10409,11 @@
         <v>14</v>
       </c>
       <c r="I184" s="9" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="J184" s="9"/>
     </row>
-    <row r="185" spans="1:10" ht="18" customHeight="1">
+    <row r="185" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" s="30" t="s">
         <v>344</v>
       </c>
@@ -10442,10 +10439,10 @@
         <v>14</v>
       </c>
       <c r="I185" s="77" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="186" spans="1:10" ht="18" customHeight="1">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" s="65" t="s">
         <v>440</v>
       </c>
@@ -10475,7 +10472,7 @@
       </c>
       <c r="J186" s="51"/>
     </row>
-    <row r="187" spans="1:10" ht="18" customHeight="1">
+    <row r="187" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" s="65" t="s">
         <v>442</v>
       </c>
@@ -10505,7 +10502,7 @@
       </c>
       <c r="J187" s="51"/>
     </row>
-    <row r="188" spans="1:10" ht="18" customHeight="1">
+    <row r="188" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A188" s="65" t="s">
         <v>445</v>
       </c>
@@ -10531,11 +10528,11 @@
         <v>14</v>
       </c>
       <c r="I188" s="52" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="J188" s="51"/>
     </row>
-    <row r="189" spans="1:10" ht="18" customHeight="1">
+    <row r="189" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A189" s="30" t="s">
         <v>447</v>
       </c>
@@ -10561,10 +10558,10 @@
         <v>14</v>
       </c>
       <c r="I189" s="54" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="190" spans="1:10" ht="18" customHeight="1">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A190" s="65" t="s">
         <v>440</v>
       </c>
@@ -10590,11 +10587,11 @@
         <v>14</v>
       </c>
       <c r="I190" s="62" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="J190" s="51"/>
     </row>
-    <row r="191" spans="1:10" ht="18" customHeight="1">
+    <row r="191" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A191" s="65" t="s">
         <v>449</v>
       </c>
@@ -10620,11 +10617,11 @@
         <v>14</v>
       </c>
       <c r="I191" s="62" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="J191" s="51"/>
     </row>
-    <row r="192" spans="1:10" ht="18" customHeight="1">
+    <row r="192" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" s="65" t="s">
         <v>377</v>
       </c>
@@ -10654,7 +10651,7 @@
       </c>
       <c r="J192" s="51"/>
     </row>
-    <row r="193" spans="1:10" ht="18" customHeight="1">
+    <row r="193" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" s="65" t="s">
         <v>276</v>
       </c>
@@ -10679,7 +10676,7 @@
       </c>
       <c r="J193" s="51"/>
     </row>
-    <row r="194" spans="1:10" ht="18" customHeight="1">
+    <row r="194" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A194" s="65" t="s">
         <v>133</v>
       </c>
@@ -10705,11 +10702,11 @@
         <v>14</v>
       </c>
       <c r="I194" s="59" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="J194" s="51"/>
     </row>
-    <row r="195" spans="1:10" ht="18" customHeight="1">
+    <row r="195" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A195" s="65" t="s">
         <v>455</v>
       </c>
@@ -10735,11 +10732,11 @@
         <v>14</v>
       </c>
       <c r="I195" s="54" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="J195" s="51"/>
     </row>
-    <row r="196" spans="1:10" ht="18" customHeight="1">
+    <row r="196" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" s="65" t="s">
         <v>457</v>
       </c>
@@ -10769,7 +10766,7 @@
       </c>
       <c r="J196" s="51"/>
     </row>
-    <row r="197" spans="1:10" ht="18" customHeight="1">
+    <row r="197" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A197" s="65" t="s">
         <v>460</v>
       </c>
@@ -10799,7 +10796,7 @@
       </c>
       <c r="J197" s="51"/>
     </row>
-    <row r="198" spans="1:10" ht="18" customHeight="1">
+    <row r="198" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" s="65" t="s">
         <v>462</v>
       </c>
@@ -10829,7 +10826,7 @@
       </c>
       <c r="J198" s="51"/>
     </row>
-    <row r="199" spans="1:10" ht="18" customHeight="1">
+    <row r="199" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" s="30" t="s">
         <v>465</v>
       </c>
@@ -10858,7 +10855,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="200" spans="1:10" ht="18" customHeight="1">
+    <row r="200" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A200" s="65" t="s">
         <v>297</v>
       </c>
@@ -10884,11 +10881,11 @@
         <v>14</v>
       </c>
       <c r="I200" s="51" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="J200" s="51"/>
     </row>
-    <row r="201" spans="1:10" ht="18" customHeight="1">
+    <row r="201" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A201" s="65" t="s">
         <v>307</v>
       </c>
@@ -10918,7 +10915,7 @@
       </c>
       <c r="J201" s="51"/>
     </row>
-    <row r="202" spans="1:10" ht="18" customHeight="1">
+    <row r="202" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A202" s="65" t="s">
         <v>216</v>
       </c>
@@ -10948,7 +10945,7 @@
       </c>
       <c r="J202" s="51"/>
     </row>
-    <row r="203" spans="1:10" ht="18" customHeight="1">
+    <row r="203" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A203" s="65" t="s">
         <v>455</v>
       </c>
@@ -10978,7 +10975,7 @@
       </c>
       <c r="J203" s="51"/>
     </row>
-    <row r="204" spans="1:10" ht="18" customHeight="1">
+    <row r="204" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A204" s="65" t="s">
         <v>474</v>
       </c>
@@ -11008,7 +11005,7 @@
       </c>
       <c r="J204" s="51"/>
     </row>
-    <row r="205" spans="1:10" ht="18" customHeight="1">
+    <row r="205" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A205" s="65" t="s">
         <v>477</v>
       </c>
@@ -11034,7 +11031,7 @@
       </c>
       <c r="J205" s="51"/>
     </row>
-    <row r="206" spans="1:10" ht="18" customHeight="1">
+    <row r="206" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A206" s="65" t="s">
         <v>481</v>
       </c>
@@ -11064,7 +11061,7 @@
       </c>
       <c r="J206" s="51"/>
     </row>
-    <row r="207" spans="1:10" ht="18" customHeight="1">
+    <row r="207" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A207" s="65" t="s">
         <v>484</v>
       </c>
@@ -11094,7 +11091,7 @@
       </c>
       <c r="J207" s="51"/>
     </row>
-    <row r="208" spans="1:10" ht="18" customHeight="1">
+    <row r="208" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A208" s="65" t="s">
         <v>307</v>
       </c>
@@ -11124,7 +11121,7 @@
       </c>
       <c r="J208" s="51"/>
     </row>
-    <row r="209" spans="1:10" ht="18" customHeight="1">
+    <row r="209" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A209" s="65" t="s">
         <v>487</v>
       </c>
@@ -11154,7 +11151,7 @@
       </c>
       <c r="J209" s="51"/>
     </row>
-    <row r="210" spans="1:10" ht="18" customHeight="1">
+    <row r="210" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A210" s="65" t="s">
         <v>295</v>
       </c>
@@ -11184,7 +11181,7 @@
       </c>
       <c r="J210" s="51"/>
     </row>
-    <row r="211" spans="1:10" ht="18" customHeight="1">
+    <row r="211" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A211" s="65" t="s">
         <v>492</v>
       </c>
@@ -11210,11 +11207,11 @@
         <v>14</v>
       </c>
       <c r="I211" s="51" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="J211" s="51"/>
     </row>
-    <row r="212" spans="1:10" ht="18" customHeight="1">
+    <row r="212" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A212" s="65" t="s">
         <v>25</v>
       </c>
@@ -11244,7 +11241,7 @@
       </c>
       <c r="J212" s="51"/>
     </row>
-    <row r="213" spans="1:10" ht="18" customHeight="1">
+    <row r="213" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A213" s="65" t="s">
         <v>25</v>
       </c>
@@ -11270,11 +11267,11 @@
         <v>14</v>
       </c>
       <c r="I213" s="51" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="J213" s="51"/>
     </row>
-    <row r="214" spans="1:10" ht="18" customHeight="1">
+    <row r="214" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A214" s="65" t="s">
         <v>497</v>
       </c>
@@ -11300,11 +11297,11 @@
         <v>14</v>
       </c>
       <c r="I214" s="51" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="J214" s="51"/>
     </row>
-    <row r="215" spans="1:10" ht="18" customHeight="1">
+    <row r="215" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A215" s="65" t="s">
         <v>492</v>
       </c>
@@ -11330,11 +11327,11 @@
         <v>14</v>
       </c>
       <c r="I215" s="51" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="J215" s="51"/>
     </row>
-    <row r="216" spans="1:10" ht="18" customHeight="1">
+    <row r="216" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A216" s="65" t="s">
         <v>499</v>
       </c>
@@ -11360,11 +11357,11 @@
         <v>14</v>
       </c>
       <c r="I216" s="51" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="J216" s="51"/>
     </row>
-    <row r="217" spans="1:10" ht="18" customHeight="1">
+    <row r="217" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A217" s="65" t="s">
         <v>501</v>
       </c>
@@ -11394,7 +11391,7 @@
       </c>
       <c r="J217" s="51"/>
     </row>
-    <row r="218" spans="1:10" ht="18" customHeight="1">
+    <row r="218" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A218" s="65" t="s">
         <v>505</v>
       </c>
@@ -11422,7 +11419,7 @@
       </c>
       <c r="J218" s="51"/>
     </row>
-    <row r="219" spans="1:10" ht="18" customHeight="1">
+    <row r="219" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A219" s="65" t="s">
         <v>507</v>
       </c>
@@ -11452,7 +11449,7 @@
       </c>
       <c r="J219" s="51"/>
     </row>
-    <row r="220" spans="1:10" ht="18" customHeight="1">
+    <row r="220" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A220" s="65" t="s">
         <v>510</v>
       </c>
@@ -11482,7 +11479,7 @@
       </c>
       <c r="J220" s="51"/>
     </row>
-    <row r="221" spans="1:10" ht="18" customHeight="1">
+    <row r="221" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A221" s="65" t="s">
         <v>514</v>
       </c>
@@ -11512,7 +11509,7 @@
       </c>
       <c r="J221" s="51"/>
     </row>
-    <row r="222" spans="1:10" ht="18" customHeight="1">
+    <row r="222" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A222" s="65" t="s">
         <v>515</v>
       </c>
@@ -11535,7 +11532,7 @@
       <c r="I222" s="51"/>
       <c r="J222" s="51"/>
     </row>
-    <row r="223" spans="1:10" ht="18" customHeight="1">
+    <row r="223" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A223" s="65" t="s">
         <v>457</v>
       </c>
@@ -11561,7 +11558,7 @@
       <c r="I223" s="51"/>
       <c r="J223" s="51"/>
     </row>
-    <row r="224" spans="1:10" ht="18" customHeight="1">
+    <row r="224" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A224" s="65" t="s">
         <v>517</v>
       </c>
@@ -11589,7 +11586,7 @@
       </c>
       <c r="J224" s="51"/>
     </row>
-    <row r="225" spans="1:10" ht="18" customHeight="1">
+    <row r="225" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A225" s="65" t="s">
         <v>520</v>
       </c>
@@ -11619,7 +11616,7 @@
       </c>
       <c r="J225" s="51"/>
     </row>
-    <row r="226" spans="1:10" ht="18" customHeight="1">
+    <row r="226" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A226" s="65" t="s">
         <v>64</v>
       </c>
@@ -11649,7 +11646,7 @@
       </c>
       <c r="J226" s="51"/>
     </row>
-    <row r="227" spans="1:10" ht="18" customHeight="1">
+    <row r="227" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A227" s="65" t="s">
         <v>525</v>
       </c>
@@ -11679,7 +11676,7 @@
       </c>
       <c r="J227" s="51"/>
     </row>
-    <row r="228" spans="1:10" ht="18" customHeight="1">
+    <row r="228" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A228" s="65" t="s">
         <v>44</v>
       </c>
@@ -11709,7 +11706,7 @@
       </c>
       <c r="J228" s="51"/>
     </row>
-    <row r="229" spans="1:10" ht="18" customHeight="1">
+    <row r="229" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A229" s="65" t="s">
         <v>270</v>
       </c>
@@ -11739,7 +11736,7 @@
       </c>
       <c r="J229" s="51"/>
     </row>
-    <row r="230" spans="1:10" ht="18" customHeight="1">
+    <row r="230" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A230" s="65" t="s">
         <v>531</v>
       </c>
@@ -11769,7 +11766,7 @@
       </c>
       <c r="J230" s="51"/>
     </row>
-    <row r="231" spans="1:10" ht="18" customHeight="1">
+    <row r="231" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A231" s="65" t="s">
         <v>532</v>
       </c>
@@ -11799,7 +11796,7 @@
       </c>
       <c r="J231" s="51"/>
     </row>
-    <row r="232" spans="1:10" ht="18" customHeight="1">
+    <row r="232" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A232" s="65" t="s">
         <v>534</v>
       </c>
@@ -11829,7 +11826,7 @@
       </c>
       <c r="J232" s="51"/>
     </row>
-    <row r="233" spans="1:10" ht="18" customHeight="1">
+    <row r="233" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A233" s="65" t="s">
         <v>525</v>
       </c>
@@ -11859,7 +11856,7 @@
       </c>
       <c r="J233" s="51"/>
     </row>
-    <row r="234" spans="1:10" ht="20" customHeight="1">
+    <row r="234" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A234" s="65" t="s">
         <v>538</v>
       </c>
@@ -11889,7 +11886,7 @@
       </c>
       <c r="J234" s="51"/>
     </row>
-    <row r="235" spans="1:10" ht="18" customHeight="1">
+    <row r="235" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A235" s="65" t="s">
         <v>541</v>
       </c>
@@ -11919,7 +11916,7 @@
       </c>
       <c r="J235" s="51"/>
     </row>
-    <row r="236" spans="1:10" ht="18" customHeight="1">
+    <row r="236" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A236" s="65" t="s">
         <v>544</v>
       </c>
@@ -11949,7 +11946,7 @@
       </c>
       <c r="J236" s="51"/>
     </row>
-    <row r="237" spans="1:10" ht="18" customHeight="1">
+    <row r="237" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A237" s="65" t="s">
         <v>546</v>
       </c>
@@ -11979,7 +11976,7 @@
       </c>
       <c r="J237" s="51"/>
     </row>
-    <row r="238" spans="1:10" ht="18" customHeight="1">
+    <row r="238" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A238" s="65" t="s">
         <v>549</v>
       </c>
@@ -12005,11 +12002,11 @@
         <v>14</v>
       </c>
       <c r="I238" s="51" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="J238" s="51"/>
     </row>
-    <row r="239" spans="1:10" ht="18" customHeight="1">
+    <row r="239" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A239" s="65" t="s">
         <v>550</v>
       </c>
@@ -12039,7 +12036,7 @@
       </c>
       <c r="J239" s="51"/>
     </row>
-    <row r="240" spans="1:10" ht="18" customHeight="1">
+    <row r="240" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A240" s="65" t="s">
         <v>525</v>
       </c>
@@ -12069,7 +12066,7 @@
       </c>
       <c r="J240" s="51"/>
     </row>
-    <row r="241" spans="1:10" ht="18" customHeight="1">
+    <row r="241" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A241" s="65" t="s">
         <v>201</v>
       </c>
@@ -12099,7 +12096,7 @@
       </c>
       <c r="J241" s="51"/>
     </row>
-    <row r="242" spans="1:10" ht="18" customHeight="1">
+    <row r="242" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A242" s="65" t="s">
         <v>553</v>
       </c>
@@ -12129,7 +12126,7 @@
       </c>
       <c r="J242" s="51"/>
     </row>
-    <row r="243" spans="1:10" ht="18" customHeight="1">
+    <row r="243" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A243" s="65" t="s">
         <v>556</v>
       </c>
@@ -12159,7 +12156,7 @@
       </c>
       <c r="J243" s="51"/>
     </row>
-    <row r="244" spans="1:10" ht="18" customHeight="1">
+    <row r="244" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A244" s="65" t="s">
         <v>559</v>
       </c>
@@ -12189,7 +12186,7 @@
       </c>
       <c r="J244" s="51"/>
     </row>
-    <row r="245" spans="1:10" ht="18" customHeight="1">
+    <row r="245" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A245" s="65" t="s">
         <v>276</v>
       </c>
@@ -12219,7 +12216,7 @@
       </c>
       <c r="J245" s="51"/>
     </row>
-    <row r="246" spans="1:10" ht="18" customHeight="1">
+    <row r="246" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A246" s="65" t="s">
         <v>565</v>
       </c>
@@ -12240,7 +12237,7 @@
       <c r="I246" s="51"/>
       <c r="J246" s="51"/>
     </row>
-    <row r="247" spans="1:10" ht="18" customHeight="1">
+    <row r="247" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A247" s="65" t="s">
         <v>566</v>
       </c>
@@ -12261,7 +12258,7 @@
       <c r="I247" s="51"/>
       <c r="J247" s="51"/>
     </row>
-    <row r="248" spans="1:10" ht="18" customHeight="1">
+    <row r="248" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A248" s="65" t="s">
         <v>568</v>
       </c>
@@ -12291,7 +12288,7 @@
       </c>
       <c r="J248" s="51"/>
     </row>
-    <row r="249" spans="1:10" ht="18" customHeight="1">
+    <row r="249" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A249" s="65" t="s">
         <v>133</v>
       </c>
@@ -12321,7 +12318,7 @@
       </c>
       <c r="J249" s="51"/>
     </row>
-    <row r="250" spans="1:10" ht="18" customHeight="1">
+    <row r="250" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A250" s="65" t="s">
         <v>573</v>
       </c>
@@ -12344,7 +12341,7 @@
       </c>
       <c r="J250" s="51"/>
     </row>
-    <row r="251" spans="1:10" ht="18" customHeight="1">
+    <row r="251" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A251" s="65" t="s">
         <v>276</v>
       </c>
@@ -12374,7 +12371,7 @@
       </c>
       <c r="J251" s="51"/>
     </row>
-    <row r="252" spans="1:10" ht="18" customHeight="1">
+    <row r="252" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A252" s="65" t="s">
         <v>344</v>
       </c>
@@ -12398,7 +12395,7 @@
       </c>
       <c r="J252" s="51"/>
     </row>
-    <row r="253" spans="1:10" ht="18" customHeight="1">
+    <row r="253" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A253" s="65" t="s">
         <v>307</v>
       </c>
@@ -12428,7 +12425,7 @@
       </c>
       <c r="J253" s="51"/>
     </row>
-    <row r="254" spans="1:10" ht="18" customHeight="1">
+    <row r="254" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A254" s="65" t="s">
         <v>581</v>
       </c>
@@ -12454,11 +12451,11 @@
         <v>14</v>
       </c>
       <c r="I254" s="51" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="J254" s="51"/>
     </row>
-    <row r="255" spans="1:10" ht="18" customHeight="1">
+    <row r="255" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A255" s="70" t="s">
         <v>583</v>
       </c>
@@ -12484,11 +12481,11 @@
         <v>14</v>
       </c>
       <c r="I255" s="62" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="J255" s="62"/>
     </row>
-    <row r="256" spans="1:10" ht="18" customHeight="1">
+    <row r="256" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A256" s="65" t="s">
         <v>44</v>
       </c>
@@ -12518,7 +12515,7 @@
       </c>
       <c r="J256" s="51"/>
     </row>
-    <row r="257" spans="1:10" ht="18" customHeight="1">
+    <row r="257" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A257" s="65" t="s">
         <v>589</v>
       </c>
@@ -12548,7 +12545,7 @@
       </c>
       <c r="J257" s="51"/>
     </row>
-    <row r="258" spans="1:10" ht="18" customHeight="1">
+    <row r="258" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A258" s="30" t="s">
         <v>593</v>
       </c>
@@ -12577,7 +12574,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="259" spans="1:10" ht="18" customHeight="1">
+    <row r="259" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A259" s="65" t="s">
         <v>597</v>
       </c>
@@ -12607,7 +12604,7 @@
       </c>
       <c r="J259" s="51"/>
     </row>
-    <row r="260" spans="1:10" ht="18" customHeight="1">
+    <row r="260" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A260" s="65" t="s">
         <v>599</v>
       </c>
@@ -12635,7 +12632,7 @@
       </c>
       <c r="J260" s="51"/>
     </row>
-    <row r="261" spans="1:10" ht="18" customHeight="1">
+    <row r="261" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A261" s="65" t="s">
         <v>601</v>
       </c>
@@ -12659,7 +12656,7 @@
       </c>
       <c r="J261" s="51"/>
     </row>
-    <row r="262" spans="1:10" ht="18" customHeight="1">
+    <row r="262" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A262" s="65" t="s">
         <v>118</v>
       </c>
@@ -12689,7 +12686,7 @@
       </c>
       <c r="J262" s="51"/>
     </row>
-    <row r="263" spans="1:10" ht="18" customHeight="1">
+    <row r="263" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A263" s="65" t="s">
         <v>531</v>
       </c>
@@ -12719,7 +12716,7 @@
       </c>
       <c r="J263" s="51"/>
     </row>
-    <row r="264" spans="1:10" ht="18" customHeight="1">
+    <row r="264" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A264" s="65" t="s">
         <v>307</v>
       </c>
@@ -12749,7 +12746,7 @@
       </c>
       <c r="J264" s="51"/>
     </row>
-    <row r="265" spans="1:10" ht="18" customHeight="1">
+    <row r="265" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A265" s="65" t="s">
         <v>609</v>
       </c>
@@ -12779,7 +12776,7 @@
       </c>
       <c r="J265" s="51"/>
     </row>
-    <row r="266" spans="1:10" ht="18" customHeight="1">
+    <row r="266" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A266" s="65" t="s">
         <v>276</v>
       </c>
@@ -12809,7 +12806,7 @@
       </c>
       <c r="J266" s="51"/>
     </row>
-    <row r="267" spans="1:10" ht="18" customHeight="1">
+    <row r="267" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A267" s="8" t="s">
         <v>289</v>
       </c>
@@ -12835,7 +12832,7 @@
       </c>
       <c r="J267" s="75"/>
     </row>
-    <row r="268" spans="1:10" ht="18" customHeight="1">
+    <row r="268" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A268" s="65" t="s">
         <v>614</v>
       </c>
@@ -12861,7 +12858,7 @@
       </c>
       <c r="J268" s="51"/>
     </row>
-    <row r="269" spans="1:10" ht="18" customHeight="1">
+    <row r="269" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A269" s="65" t="s">
         <v>440</v>
       </c>
@@ -12887,7 +12884,7 @@
       </c>
       <c r="J269" s="51"/>
     </row>
-    <row r="270" spans="1:10" ht="18" customHeight="1">
+    <row r="270" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A270" s="65" t="s">
         <v>617</v>
       </c>
@@ -12913,7 +12910,7 @@
       </c>
       <c r="J270" s="51"/>
     </row>
-    <row r="271" spans="1:10" ht="18" customHeight="1">
+    <row r="271" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A271" s="65" t="s">
         <v>39</v>
       </c>
@@ -12941,7 +12938,7 @@
       </c>
       <c r="J271" s="51"/>
     </row>
-    <row r="272" spans="1:10" ht="18" customHeight="1">
+    <row r="272" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A272" s="65" t="s">
         <v>620</v>
       </c>
@@ -12969,7 +12966,7 @@
       </c>
       <c r="J272" s="51"/>
     </row>
-    <row r="273" spans="1:10" ht="18" customHeight="1">
+    <row r="273" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A273" s="65" t="s">
         <v>622</v>
       </c>
@@ -12995,7 +12992,7 @@
       </c>
       <c r="J273" s="51"/>
     </row>
-    <row r="274" spans="1:10" ht="18" customHeight="1">
+    <row r="274" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A274" s="65" t="s">
         <v>624</v>
       </c>
@@ -13021,7 +13018,7 @@
       </c>
       <c r="J274" s="51"/>
     </row>
-    <row r="275" spans="1:10" ht="18" customHeight="1">
+    <row r="275" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A275" s="65" t="s">
         <v>626</v>
       </c>
@@ -13049,7 +13046,7 @@
       </c>
       <c r="J275" s="51"/>
     </row>
-    <row r="276" spans="1:10" ht="18" customHeight="1">
+    <row r="276" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A276" s="65" t="s">
         <v>276</v>
       </c>
@@ -13075,7 +13072,7 @@
       </c>
       <c r="J276" s="51"/>
     </row>
-    <row r="277" spans="1:10" ht="18" customHeight="1">
+    <row r="277" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A277" s="65" t="s">
         <v>629</v>
       </c>
@@ -13101,7 +13098,7 @@
       </c>
       <c r="J277" s="51"/>
     </row>
-    <row r="278" spans="1:10" ht="18" customHeight="1">
+    <row r="278" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A278" s="65" t="s">
         <v>633</v>
       </c>
@@ -13127,7 +13124,7 @@
       </c>
       <c r="J278" s="51"/>
     </row>
-    <row r="279" spans="1:10" ht="18" customHeight="1">
+    <row r="279" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A279" s="65" t="s">
         <v>635</v>
       </c>
@@ -13153,7 +13150,7 @@
       </c>
       <c r="J279" s="51"/>
     </row>
-    <row r="280" spans="1:10" ht="18" customHeight="1">
+    <row r="280" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A280" s="65" t="s">
         <v>609</v>
       </c>
@@ -13179,7 +13176,7 @@
       </c>
       <c r="J280" s="51"/>
     </row>
-    <row r="281" spans="1:10" ht="18" customHeight="1">
+    <row r="281" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A281" s="8" t="s">
         <v>638</v>
       </c>
@@ -13205,7 +13202,7 @@
       </c>
       <c r="J281" s="75"/>
     </row>
-    <row r="282" spans="1:10" ht="18" customHeight="1">
+    <row r="282" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A282" s="65" t="s">
         <v>635</v>
       </c>
@@ -13229,7 +13226,7 @@
       <c r="I282" s="51"/>
       <c r="J282" s="51"/>
     </row>
-    <row r="283" spans="1:10" ht="18" customHeight="1">
+    <row r="283" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A283" s="65" t="s">
         <v>641</v>
       </c>
@@ -13253,7 +13250,7 @@
       <c r="I283" s="51"/>
       <c r="J283" s="51"/>
     </row>
-    <row r="284" spans="1:10" ht="18" customHeight="1">
+    <row r="284" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A284" s="65" t="s">
         <v>263</v>
       </c>
@@ -13277,7 +13274,7 @@
       <c r="I284" s="51"/>
       <c r="J284" s="51"/>
     </row>
-    <row r="285" spans="1:10" ht="18" customHeight="1">
+    <row r="285" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A285" s="8" t="s">
         <v>644</v>
       </c>
@@ -13303,7 +13300,7 @@
       </c>
       <c r="J285" s="75"/>
     </row>
-    <row r="286" spans="1:10" ht="18" customHeight="1">
+    <row r="286" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A286" s="8" t="s">
         <v>644</v>
       </c>
@@ -13327,7 +13324,7 @@
       <c r="I286" s="75"/>
       <c r="J286" s="75"/>
     </row>
-    <row r="287" spans="1:10" ht="18" customHeight="1">
+    <row r="287" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A287" s="65" t="s">
         <v>170</v>
       </c>
@@ -13351,7 +13348,7 @@
       </c>
       <c r="J287" s="51"/>
     </row>
-    <row r="288" spans="1:10" ht="18" customHeight="1">
+    <row r="288" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A288" s="65" t="s">
         <v>170</v>
       </c>
@@ -13375,7 +13372,7 @@
       <c r="I288" s="51"/>
       <c r="J288" s="51"/>
     </row>
-    <row r="289" spans="1:10" ht="18" customHeight="1">
+    <row r="289" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A289" s="65" t="s">
         <v>652</v>
       </c>
@@ -13399,7 +13396,7 @@
       </c>
       <c r="J289" s="51"/>
     </row>
-    <row r="290" spans="1:10">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A290" s="54" t="s">
         <v>225</v>
       </c>
@@ -13431,13 +13428,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E61C4E4-BEB5-45C3-ABA5-D05E41F83072}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
@@ -13446,13 +13443,12 @@
     <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="9.1796875" customWidth="1"/>
+    <col min="8" max="8" width="29.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1">
+    <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
@@ -13474,13 +13470,10 @@
       <c r="G1" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="76" t="s">
-        <v>658</v>
-      </c>
-      <c r="I1" s="49" t="s">
+      <c r="H1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="I1" s="46" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: Update the report generation validations
</commit_message>
<xml_diff>
--- a/Data/Temp/TransactionStatus.xlsx
+++ b/Data/Temp/TransactionStatus.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\UiPath\Fast_Pipe_Automation\Data\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FredrickMutua\Documents\UiPath\FastPipe_Automation\Data\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2E918A-2DC5-4CAB-9513-DF2F898ECCFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4961C444-4788-43D4-AD23-E4A826CBCC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Successful" sheetId="3" r:id="rId1"/>
@@ -6039,27 +6039,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DED64C-ED90-4504-A3DE-AF1F5E294B87}">
   <dimension ref="A1:J289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A266" zoomScale="47" zoomScaleNormal="47" workbookViewId="0">
-      <selection activeCell="D284" sqref="D284"/>
+    <sheetView tabSelected="1" zoomScale="47" zoomScaleNormal="47" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="24.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.36328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="255" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7265625" style="11" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="11"/>
+    <col min="10" max="10" width="3.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" style="11" customWidth="1"/>
+    <col min="12" max="16384" width="8.7109375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" ht="18.75">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -6089,7 +6089,7 @@
       </c>
       <c r="J1" s="30"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" ht="18.75">
       <c r="A2" s="28" t="s">
         <v>9</v>
       </c>
@@ -6119,7 +6119,7 @@
       </c>
       <c r="J2" s="35"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" ht="18.75">
       <c r="A3" s="28" t="s">
         <v>15</v>
       </c>
@@ -6147,7 +6147,7 @@
       </c>
       <c r="J3" s="35"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" ht="18.75">
       <c r="A4" s="28" t="s">
         <v>20</v>
       </c>
@@ -6175,7 +6175,7 @@
       </c>
       <c r="J4" s="35"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" ht="18.75">
       <c r="A5" s="28" t="s">
         <v>25</v>
       </c>
@@ -6205,7 +6205,7 @@
       </c>
       <c r="J5" s="36"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" ht="18.75">
       <c r="A6" s="28" t="s">
         <v>30</v>
       </c>
@@ -6233,7 +6233,7 @@
       </c>
       <c r="J6" s="35"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" ht="18.75">
       <c r="A7" s="28" t="s">
         <v>35</v>
       </c>
@@ -6261,7 +6261,7 @@
       </c>
       <c r="J7" s="35"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" ht="18.75">
       <c r="A8" s="28" t="s">
         <v>39</v>
       </c>
@@ -6289,7 +6289,7 @@
       </c>
       <c r="J8" s="35"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" ht="18.75">
       <c r="A9" s="28" t="s">
         <v>44</v>
       </c>
@@ -6317,7 +6317,7 @@
       </c>
       <c r="J9" s="35"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="18.75">
       <c r="A10" s="28" t="s">
         <v>49</v>
       </c>
@@ -6345,7 +6345,7 @@
       </c>
       <c r="J10" s="36"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" ht="18.75">
       <c r="A11" s="28" t="s">
         <v>54</v>
       </c>
@@ -6373,7 +6373,7 @@
       </c>
       <c r="J11" s="35"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" ht="18.75">
       <c r="A12" s="28" t="s">
         <v>58</v>
       </c>
@@ -6401,7 +6401,7 @@
       </c>
       <c r="J12" s="41"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" ht="18.75">
       <c r="A13" s="28" t="s">
         <v>60</v>
       </c>
@@ -6429,7 +6429,7 @@
       </c>
       <c r="J13" s="35"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" ht="18.75">
       <c r="A14" s="28" t="s">
         <v>64</v>
       </c>
@@ -6457,7 +6457,7 @@
       </c>
       <c r="J14" s="35"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" ht="18.75">
       <c r="A15" s="28" t="s">
         <v>66</v>
       </c>
@@ -6485,7 +6485,7 @@
       </c>
       <c r="J15" s="35"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" ht="18.75">
       <c r="A16" s="28" t="s">
         <v>68</v>
       </c>
@@ -6513,7 +6513,7 @@
       </c>
       <c r="J16" s="35"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" ht="18.75">
       <c r="A17" s="28" t="s">
         <v>44</v>
       </c>
@@ -6541,7 +6541,7 @@
       </c>
       <c r="J17" s="35"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" ht="18.75">
       <c r="A18" s="28" t="s">
         <v>71</v>
       </c>
@@ -6569,7 +6569,7 @@
       </c>
       <c r="J18" s="35"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" ht="18.75">
       <c r="A19" s="42" t="s">
         <v>35</v>
       </c>
@@ -6597,7 +6597,7 @@
       </c>
       <c r="J19" s="35"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" ht="18.75">
       <c r="A20" s="28" t="s">
         <v>77</v>
       </c>
@@ -6625,7 +6625,7 @@
       </c>
       <c r="J20" s="35"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" ht="18.75">
       <c r="A21" s="28" t="s">
         <v>81</v>
       </c>
@@ -6653,7 +6653,7 @@
       </c>
       <c r="J21" s="35"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" ht="18.75">
       <c r="A22" s="28" t="s">
         <v>83</v>
       </c>
@@ -6681,7 +6681,7 @@
       </c>
       <c r="J22" s="35"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" ht="18.75">
       <c r="A23" s="28" t="s">
         <v>86</v>
       </c>
@@ -6709,7 +6709,7 @@
       </c>
       <c r="J23" s="35"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" ht="18.75">
       <c r="A24" s="28" t="s">
         <v>89</v>
       </c>
@@ -6737,7 +6737,7 @@
       </c>
       <c r="J24" s="35"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" ht="18.75">
       <c r="A25" s="28" t="s">
         <v>93</v>
       </c>
@@ -6765,7 +6765,7 @@
       </c>
       <c r="J25" s="35"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" ht="18.75">
       <c r="A26" s="46" t="s">
         <v>95</v>
       </c>
@@ -6795,7 +6795,7 @@
       </c>
       <c r="J26" s="35"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" ht="18.75">
       <c r="A27" s="28" t="s">
         <v>98</v>
       </c>
@@ -6823,7 +6823,7 @@
       </c>
       <c r="J27" s="35"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" ht="18.75">
       <c r="A28" s="28" t="s">
         <v>100</v>
       </c>
@@ -6851,7 +6851,7 @@
       </c>
       <c r="J28" s="35"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" ht="18.75">
       <c r="A29" s="28" t="s">
         <v>103</v>
       </c>
@@ -6879,7 +6879,7 @@
       </c>
       <c r="J29" s="35"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" ht="18.75">
       <c r="A30" s="46" t="s">
         <v>106</v>
       </c>
@@ -6907,7 +6907,7 @@
       </c>
       <c r="J30" s="35"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" ht="18.75">
       <c r="A31" s="28" t="s">
         <v>110</v>
       </c>
@@ -6935,7 +6935,7 @@
       </c>
       <c r="J31" s="36"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" ht="18.75">
       <c r="A32" s="46" t="s">
         <v>114</v>
       </c>
@@ -6965,7 +6965,7 @@
       </c>
       <c r="J32" s="36"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" ht="18.75">
       <c r="A33" s="28" t="s">
         <v>114</v>
       </c>
@@ -6995,7 +6995,7 @@
       </c>
       <c r="J33" s="36"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" ht="18.75">
       <c r="A34" s="28" t="s">
         <v>120</v>
       </c>
@@ -7023,7 +7023,7 @@
       </c>
       <c r="J34" s="36"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" ht="18.75">
       <c r="A35" s="28" t="s">
         <v>124</v>
       </c>
@@ -7053,7 +7053,7 @@
       </c>
       <c r="J35" s="36"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" ht="18.75">
       <c r="A36" s="28" t="s">
         <v>129</v>
       </c>
@@ -7081,7 +7081,7 @@
       </c>
       <c r="J36" s="36"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" ht="18.75">
       <c r="A37" s="28" t="s">
         <v>132</v>
       </c>
@@ -7109,7 +7109,7 @@
       </c>
       <c r="J37" s="35"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" ht="18.75">
       <c r="A38" s="28" t="s">
         <v>135</v>
       </c>
@@ -7137,7 +7137,7 @@
       </c>
       <c r="J38" s="35"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" ht="18.75">
       <c r="A39" s="28" t="s">
         <v>137</v>
       </c>
@@ -7165,7 +7165,7 @@
       </c>
       <c r="J39" s="35"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" ht="18.75">
       <c r="A40" s="28" t="s">
         <v>141</v>
       </c>
@@ -7193,7 +7193,7 @@
       </c>
       <c r="J40" s="35"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" ht="18.75">
       <c r="A41" s="28" t="s">
         <v>144</v>
       </c>
@@ -7221,7 +7221,7 @@
       </c>
       <c r="J41" s="40"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" ht="18.75">
       <c r="A42" s="28" t="s">
         <v>147</v>
       </c>
@@ -7251,7 +7251,7 @@
       </c>
       <c r="J42" s="53"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" ht="18.75">
       <c r="A43" s="28" t="s">
         <v>152</v>
       </c>
@@ -7281,7 +7281,7 @@
       </c>
       <c r="J43" s="53"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" ht="18.75">
       <c r="A44" s="28" t="s">
         <v>155</v>
       </c>
@@ -7311,7 +7311,7 @@
       </c>
       <c r="J44" s="53"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" ht="18.75">
       <c r="A45" s="28" t="s">
         <v>159</v>
       </c>
@@ -7341,7 +7341,7 @@
       </c>
       <c r="J45" s="53"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" ht="18.75">
       <c r="A46" s="28" t="s">
         <v>163</v>
       </c>
@@ -7371,7 +7371,7 @@
       </c>
       <c r="J46" s="53"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" ht="18.75">
       <c r="A47" s="28" t="s">
         <v>168</v>
       </c>
@@ -7401,7 +7401,7 @@
       </c>
       <c r="J47" s="53"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" ht="18.75">
       <c r="A48" s="54"/>
       <c r="B48" s="55" t="s">
         <v>16</v>
@@ -7429,7 +7429,7 @@
       </c>
       <c r="J48" s="53"/>
     </row>
-    <row r="49" spans="1:10" ht="20" customHeight="1">
+    <row r="49" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="28" t="s">
         <v>114</v>
       </c>
@@ -7459,7 +7459,7 @@
       </c>
       <c r="J49" s="53"/>
     </row>
-    <row r="50" spans="1:10" ht="20" customHeight="1">
+    <row r="50" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="28" t="s">
         <v>177</v>
       </c>
@@ -7489,7 +7489,7 @@
       </c>
       <c r="J50" s="53"/>
     </row>
-    <row r="51" spans="1:10" ht="20" customHeight="1">
+    <row r="51" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="28" t="s">
         <v>181</v>
       </c>
@@ -7579,7 +7579,7 @@
       </c>
       <c r="J53" s="53"/>
     </row>
-    <row r="54" spans="1:10" ht="20" customHeight="1">
+    <row r="54" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A54" s="28" t="s">
         <v>120</v>
       </c>
@@ -7609,7 +7609,7 @@
       </c>
       <c r="J54" s="53"/>
     </row>
-    <row r="55" spans="1:10" ht="20" customHeight="1">
+    <row r="55" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A55" s="28" t="s">
         <v>192</v>
       </c>
@@ -7639,7 +7639,7 @@
       </c>
       <c r="J55" s="53"/>
     </row>
-    <row r="56" spans="1:10" ht="20" customHeight="1">
+    <row r="56" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A56" s="28" t="s">
         <v>196</v>
       </c>
@@ -7669,7 +7669,7 @@
       </c>
       <c r="J56" s="53"/>
     </row>
-    <row r="57" spans="1:10" ht="20" customHeight="1">
+    <row r="57" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A57" s="28" t="s">
         <v>198</v>
       </c>
@@ -7699,7 +7699,7 @@
       </c>
       <c r="J57" s="53"/>
     </row>
-    <row r="58" spans="1:10" ht="20" customHeight="1">
+    <row r="58" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A58" s="28" t="s">
         <v>201</v>
       </c>
@@ -7729,7 +7729,7 @@
       </c>
       <c r="J58" s="67"/>
     </row>
-    <row r="59" spans="1:10" ht="20.5" customHeight="1">
+    <row r="59" spans="1:10" ht="20.45" customHeight="1">
       <c r="A59" s="28" t="s">
         <v>203</v>
       </c>
@@ -7759,7 +7759,7 @@
       </c>
       <c r="J59" s="53"/>
     </row>
-    <row r="60" spans="1:10" ht="20" customHeight="1">
+    <row r="60" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A60" s="28" t="s">
         <v>205</v>
       </c>
@@ -7789,7 +7789,7 @@
       </c>
       <c r="J60" s="53"/>
     </row>
-    <row r="61" spans="1:10" ht="20" customHeight="1">
+    <row r="61" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A61" s="28" t="s">
         <v>208</v>
       </c>
@@ -7819,7 +7819,7 @@
       </c>
       <c r="J61" s="53"/>
     </row>
-    <row r="62" spans="1:10" ht="20" customHeight="1">
+    <row r="62" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A62" s="28" t="s">
         <v>211</v>
       </c>
@@ -7847,7 +7847,7 @@
       <c r="I62" s="61"/>
       <c r="J62" s="53"/>
     </row>
-    <row r="63" spans="1:10" ht="20.5" customHeight="1">
+    <row r="63" spans="1:10" ht="20.45" customHeight="1">
       <c r="A63" s="28" t="s">
         <v>214</v>
       </c>
@@ -7877,7 +7877,7 @@
       </c>
       <c r="J63" s="53"/>
     </row>
-    <row r="64" spans="1:10" ht="20" customHeight="1">
+    <row r="64" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A64" s="28" t="s">
         <v>217</v>
       </c>
@@ -7907,7 +7907,7 @@
       </c>
       <c r="J64" s="53"/>
     </row>
-    <row r="65" spans="1:10" ht="20" customHeight="1">
+    <row r="65" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A65" s="46" t="s">
         <v>221</v>
       </c>
@@ -7937,7 +7937,7 @@
       </c>
       <c r="J65" s="53"/>
     </row>
-    <row r="66" spans="1:10" ht="20" customHeight="1">
+    <row r="66" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A66" s="28" t="s">
         <v>177</v>
       </c>
@@ -7967,7 +7967,7 @@
       </c>
       <c r="J66" s="53"/>
     </row>
-    <row r="67" spans="1:10" ht="20.5" customHeight="1">
+    <row r="67" spans="1:10" ht="20.45" customHeight="1">
       <c r="A67" s="28" t="s">
         <v>224</v>
       </c>
@@ -7997,7 +7997,7 @@
       </c>
       <c r="J67" s="53"/>
     </row>
-    <row r="68" spans="1:10" ht="20.5" customHeight="1">
+    <row r="68" spans="1:10" ht="20.45" customHeight="1">
       <c r="A68" s="28" t="s">
         <v>227</v>
       </c>
@@ -8027,7 +8027,7 @@
       </c>
       <c r="J68" s="67"/>
     </row>
-    <row r="69" spans="1:10" ht="20" customHeight="1">
+    <row r="69" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A69" s="46" t="s">
         <v>229</v>
       </c>
@@ -8057,7 +8057,7 @@
       </c>
       <c r="J69" s="53"/>
     </row>
-    <row r="70" spans="1:10" ht="20" customHeight="1">
+    <row r="70" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A70" s="46" t="s">
         <v>177</v>
       </c>
@@ -8087,7 +8087,7 @@
       </c>
       <c r="J70" s="53"/>
     </row>
-    <row r="71" spans="1:10" ht="20.5" customHeight="1">
+    <row r="71" spans="1:10" ht="20.45" customHeight="1">
       <c r="A71" s="28" t="s">
         <v>201</v>
       </c>
@@ -8117,7 +8117,7 @@
       </c>
       <c r="J71" s="53"/>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" ht="18.75">
       <c r="A72" s="28" t="s">
         <v>232</v>
       </c>
@@ -8147,7 +8147,7 @@
       </c>
       <c r="J72" s="53"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" ht="18.75">
       <c r="A73" s="28" t="s">
         <v>232</v>
       </c>
@@ -8177,7 +8177,7 @@
       </c>
       <c r="J73" s="53"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" ht="18.75">
       <c r="A74" s="28" t="s">
         <v>236</v>
       </c>
@@ -8207,7 +8207,7 @@
       </c>
       <c r="J74" s="53"/>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" ht="18.75">
       <c r="A75" s="28" t="s">
         <v>238</v>
       </c>
@@ -8237,7 +8237,7 @@
       </c>
       <c r="J75" s="36"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" ht="18.75">
       <c r="A76" s="28" t="s">
         <v>192</v>
       </c>
@@ -8267,7 +8267,7 @@
       </c>
       <c r="J76" s="36"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" ht="18.75">
       <c r="A77" s="28" t="s">
         <v>44</v>
       </c>
@@ -8297,7 +8297,7 @@
       </c>
       <c r="J77" s="36"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" ht="18.75">
       <c r="A78" s="28" t="s">
         <v>177</v>
       </c>
@@ -8327,7 +8327,7 @@
       </c>
       <c r="J78" s="36"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" ht="18.75">
       <c r="A79" s="28" t="s">
         <v>246</v>
       </c>
@@ -8357,7 +8357,7 @@
       </c>
       <c r="J79" s="36"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" ht="18.75">
       <c r="A80" s="28" t="s">
         <v>120</v>
       </c>
@@ -8387,7 +8387,7 @@
       </c>
       <c r="J80" s="36"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" ht="18.75">
       <c r="A81" s="28" t="s">
         <v>114</v>
       </c>
@@ -8413,7 +8413,7 @@
       <c r="I81" s="169"/>
       <c r="J81" s="36"/>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" ht="18.75">
       <c r="A82" s="28" t="s">
         <v>250</v>
       </c>
@@ -8443,7 +8443,7 @@
       </c>
       <c r="J82" s="36"/>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" ht="18.75">
       <c r="A83" s="28" t="s">
         <v>254</v>
       </c>
@@ -8473,7 +8473,7 @@
       </c>
       <c r="J83" s="36"/>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" ht="18.75">
       <c r="A84" s="28" t="s">
         <v>236</v>
       </c>
@@ -8503,7 +8503,7 @@
       </c>
       <c r="J84" s="36"/>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" ht="18.75">
       <c r="A85" s="28" t="s">
         <v>258</v>
       </c>
@@ -8533,7 +8533,7 @@
       </c>
       <c r="J85" s="36"/>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" ht="18.75">
       <c r="A86" s="28" t="s">
         <v>261</v>
       </c>
@@ -8563,7 +8563,7 @@
       </c>
       <c r="J86" s="36"/>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" ht="18.75">
       <c r="A87" s="28" t="s">
         <v>263</v>
       </c>
@@ -8593,7 +8593,7 @@
       </c>
       <c r="J87" s="36"/>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" ht="18.75">
       <c r="A88" s="28" t="s">
         <v>266</v>
       </c>
@@ -8623,7 +8623,7 @@
       </c>
       <c r="J88" s="36"/>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" ht="18.75">
       <c r="A89" s="28" t="s">
         <v>269</v>
       </c>
@@ -8653,7 +8653,7 @@
       </c>
       <c r="J89" s="36"/>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" ht="18.75">
       <c r="A90" s="28" t="s">
         <v>269</v>
       </c>
@@ -8683,7 +8683,7 @@
       </c>
       <c r="J90" s="36"/>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" ht="18.75">
       <c r="A91" s="28" t="s">
         <v>44</v>
       </c>
@@ -8713,7 +8713,7 @@
       </c>
       <c r="J91" s="36"/>
     </row>
-    <row r="92" spans="1:10" ht="20" customHeight="1">
+    <row r="92" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A92" s="28" t="s">
         <v>44</v>
       </c>
@@ -8743,7 +8743,7 @@
       </c>
       <c r="J92" s="36"/>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" ht="18.75">
       <c r="A93" s="28" t="s">
         <v>266</v>
       </c>
@@ -8771,7 +8771,7 @@
       </c>
       <c r="J93" s="36"/>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" ht="18.75">
       <c r="A94" s="28" t="s">
         <v>276</v>
       </c>
@@ -8801,7 +8801,7 @@
       </c>
       <c r="J94" s="36"/>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" ht="18.75">
       <c r="A95" s="28" t="s">
         <v>278</v>
       </c>
@@ -8831,7 +8831,7 @@
       </c>
       <c r="J95" s="36"/>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" ht="18.75">
       <c r="A96" s="28" t="s">
         <v>280</v>
       </c>
@@ -8861,7 +8861,7 @@
       </c>
       <c r="J96" s="36"/>
     </row>
-    <row r="97" spans="1:10" ht="20" customHeight="1">
+    <row r="97" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A97" s="28" t="s">
         <v>283</v>
       </c>
@@ -8891,7 +8891,7 @@
       </c>
       <c r="J97" s="36"/>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" ht="18.75">
       <c r="A98" s="28" t="s">
         <v>285</v>
       </c>
@@ -8921,7 +8921,7 @@
       </c>
       <c r="J98" s="36"/>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" ht="18.75">
       <c r="A99" s="28" t="s">
         <v>287</v>
       </c>
@@ -8951,7 +8951,7 @@
       </c>
       <c r="J99" s="53"/>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" ht="18.75">
       <c r="A100" s="28" t="s">
         <v>289</v>
       </c>
@@ -8981,7 +8981,7 @@
       </c>
       <c r="J100" s="53"/>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" ht="18.75">
       <c r="A101" s="28" t="s">
         <v>290</v>
       </c>
@@ -9011,7 +9011,7 @@
       </c>
       <c r="J101" s="36"/>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" ht="18.75">
       <c r="A102" s="28" t="s">
         <v>292</v>
       </c>
@@ -9041,7 +9041,7 @@
       </c>
       <c r="J102" s="36"/>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" ht="18.75">
       <c r="A103" s="28" t="s">
         <v>285</v>
       </c>
@@ -9071,7 +9071,7 @@
       </c>
       <c r="J103" s="36"/>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" ht="18.75">
       <c r="A104" s="28" t="s">
         <v>120</v>
       </c>
@@ -9101,7 +9101,7 @@
       </c>
       <c r="J104" s="36"/>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" ht="18.75">
       <c r="A105" s="28" t="s">
         <v>298</v>
       </c>
@@ -9131,7 +9131,7 @@
       </c>
       <c r="J105" s="35"/>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" ht="18.75">
       <c r="A106" s="28" t="s">
         <v>301</v>
       </c>
@@ -9161,7 +9161,7 @@
       </c>
       <c r="J106" s="35"/>
     </row>
-    <row r="107" spans="1:10" ht="18.5" customHeight="1">
+    <row r="107" spans="1:10" ht="18.600000000000001" customHeight="1">
       <c r="A107" s="46" t="s">
         <v>302</v>
       </c>
@@ -9191,7 +9191,7 @@
       </c>
       <c r="J107" s="35"/>
     </row>
-    <row r="108" spans="1:10" ht="18.5" customHeight="1">
+    <row r="108" spans="1:10" ht="18.600000000000001" customHeight="1">
       <c r="A108" s="28" t="s">
         <v>227</v>
       </c>
@@ -9221,7 +9221,7 @@
       </c>
       <c r="J108" s="35"/>
     </row>
-    <row r="109" spans="1:10" ht="20" customHeight="1">
+    <row r="109" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A109" s="86" t="s">
         <v>304</v>
       </c>
@@ -9251,7 +9251,7 @@
       </c>
       <c r="J109" s="37"/>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" ht="18.75">
       <c r="A110" s="46" t="s">
         <v>163</v>
       </c>
@@ -9281,7 +9281,7 @@
       </c>
       <c r="J110" s="36"/>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" ht="18.75">
       <c r="A111" s="28" t="s">
         <v>308</v>
       </c>
@@ -9311,7 +9311,7 @@
       </c>
       <c r="J111" s="36"/>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" ht="18.75">
       <c r="A112" s="28" t="s">
         <v>310</v>
       </c>
@@ -9341,7 +9341,7 @@
       </c>
       <c r="J112" s="36"/>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" ht="18.75">
       <c r="A113" s="28" t="s">
         <v>313</v>
       </c>
@@ -9371,7 +9371,7 @@
       </c>
       <c r="J113" s="36"/>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" ht="18.75">
       <c r="A114" s="46" t="s">
         <v>315</v>
       </c>
@@ -9401,7 +9401,7 @@
       </c>
       <c r="J114" s="36"/>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" ht="18.75">
       <c r="A115" s="28" t="s">
         <v>318</v>
       </c>
@@ -9431,7 +9431,7 @@
       </c>
       <c r="J115" s="36"/>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" ht="18.75">
       <c r="A116" s="28" t="s">
         <v>320</v>
       </c>
@@ -9461,7 +9461,7 @@
       </c>
       <c r="J116" s="36"/>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" ht="18.75">
       <c r="A117" s="46" t="s">
         <v>315</v>
       </c>
@@ -9491,7 +9491,7 @@
       </c>
       <c r="J117" s="36"/>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" ht="18.75">
       <c r="A118" s="28" t="s">
         <v>120</v>
       </c>
@@ -9521,7 +9521,7 @@
       </c>
       <c r="J118" s="36"/>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" ht="18.75">
       <c r="A119" s="28" t="s">
         <v>214</v>
       </c>
@@ -9551,7 +9551,7 @@
       </c>
       <c r="J119" s="36"/>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" ht="18.75">
       <c r="A120" s="28" t="s">
         <v>324</v>
       </c>
@@ -9581,7 +9581,7 @@
       </c>
       <c r="J120" s="36"/>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" ht="18.75">
       <c r="A121" s="28" t="s">
         <v>327</v>
       </c>
@@ -9608,7 +9608,7 @@
       </c>
       <c r="J121" s="53"/>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" ht="18.75">
       <c r="A122" s="28" t="s">
         <v>328</v>
       </c>
@@ -9638,7 +9638,7 @@
       </c>
       <c r="J122" s="53"/>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" ht="18.75">
       <c r="A123" s="28" t="s">
         <v>331</v>
       </c>
@@ -9668,7 +9668,7 @@
       </c>
       <c r="J123" s="53"/>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" ht="18.75">
       <c r="A124" s="28" t="s">
         <v>333</v>
       </c>
@@ -9698,7 +9698,7 @@
       </c>
       <c r="J124" s="53"/>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" ht="18.75">
       <c r="A125" s="28" t="s">
         <v>114</v>
       </c>
@@ -9728,7 +9728,7 @@
       </c>
       <c r="J125" s="53"/>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" ht="18.75">
       <c r="A126" s="28" t="s">
         <v>336</v>
       </c>
@@ -9758,7 +9758,7 @@
       </c>
       <c r="J126" s="53"/>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" ht="18.75">
       <c r="A127" s="46" t="s">
         <v>229</v>
       </c>
@@ -9788,7 +9788,7 @@
       </c>
       <c r="J127" s="36"/>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" ht="18.75">
       <c r="A128" s="46" t="s">
         <v>229</v>
       </c>
@@ -9818,7 +9818,7 @@
       </c>
       <c r="J128" s="36"/>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" ht="18.75">
       <c r="A129" s="28" t="s">
         <v>333</v>
       </c>
@@ -9848,7 +9848,7 @@
       </c>
       <c r="J129" s="36"/>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" ht="18.75">
       <c r="A130" s="28" t="s">
         <v>340</v>
       </c>
@@ -9878,7 +9878,7 @@
       </c>
       <c r="J130" s="36"/>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" ht="18.75">
       <c r="A131" s="28" t="s">
         <v>342</v>
       </c>
@@ -9908,7 +9908,7 @@
       </c>
       <c r="J131" s="36"/>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" ht="18.75">
       <c r="A132" s="28" t="s">
         <v>340</v>
       </c>
@@ -9938,7 +9938,7 @@
       </c>
       <c r="J132" s="36"/>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" ht="18.75">
       <c r="A133" s="28" t="s">
         <v>343</v>
       </c>
@@ -9968,7 +9968,7 @@
       </c>
       <c r="J133" s="36"/>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" ht="18.75">
       <c r="A134" s="28" t="s">
         <v>346</v>
       </c>
@@ -9998,7 +9998,7 @@
       </c>
       <c r="J134" s="36"/>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" ht="18.75">
       <c r="A135" s="28" t="s">
         <v>336</v>
       </c>
@@ -10028,7 +10028,7 @@
       </c>
       <c r="J135" s="53"/>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" ht="18.75">
       <c r="A136" s="28" t="s">
         <v>342</v>
       </c>
@@ -10058,7 +10058,7 @@
       </c>
       <c r="J136" s="53"/>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" ht="18.75">
       <c r="A137" s="28" t="s">
         <v>350</v>
       </c>
@@ -10088,7 +10088,7 @@
       </c>
       <c r="J137" s="53"/>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" ht="18.75">
       <c r="A138" s="28" t="s">
         <v>354</v>
       </c>
@@ -10118,7 +10118,7 @@
       </c>
       <c r="J138" s="53"/>
     </row>
-    <row r="139" spans="1:10" ht="20" customHeight="1">
+    <row r="139" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A139" s="28" t="s">
         <v>357</v>
       </c>
@@ -10148,7 +10148,7 @@
       </c>
       <c r="J139" s="53"/>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" ht="18.75">
       <c r="A140" s="28" t="s">
         <v>360</v>
       </c>
@@ -10178,7 +10178,7 @@
       </c>
       <c r="J140" s="53"/>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" ht="18.75">
       <c r="A141" s="28" t="s">
         <v>238</v>
       </c>
@@ -10208,7 +10208,7 @@
       </c>
       <c r="J141" s="53"/>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" ht="18.75">
       <c r="A142" s="28" t="s">
         <v>54</v>
       </c>
@@ -10238,7 +10238,7 @@
       </c>
       <c r="J142" s="53"/>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" ht="18.75">
       <c r="A143" s="28" t="s">
         <v>363</v>
       </c>
@@ -10268,7 +10268,7 @@
       </c>
       <c r="J143" s="53"/>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" ht="18.75">
       <c r="A144" s="46" t="s">
         <v>365</v>
       </c>
@@ -10298,7 +10298,7 @@
       </c>
       <c r="J144" s="35"/>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" ht="18.75">
       <c r="A145" s="28" t="s">
         <v>192</v>
       </c>
@@ -10326,7 +10326,7 @@
       <c r="I145" s="94"/>
       <c r="J145" s="36"/>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" ht="18.75">
       <c r="A146" s="28" t="s">
         <v>192</v>
       </c>
@@ -10354,7 +10354,7 @@
       <c r="I146" s="94"/>
       <c r="J146" s="36"/>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" ht="18.75">
       <c r="A147" s="28" t="s">
         <v>342</v>
       </c>
@@ -10384,7 +10384,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" ht="18.75">
       <c r="A148" s="28" t="s">
         <v>371</v>
       </c>
@@ -10412,7 +10412,7 @@
       <c r="I148" s="8"/>
       <c r="J148" s="36"/>
     </row>
-    <row r="149" spans="1:10" ht="20" customHeight="1">
+    <row r="149" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A149" s="28" t="s">
         <v>374</v>
       </c>
@@ -10442,7 +10442,7 @@
       </c>
       <c r="J149" s="67"/>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" ht="18.75">
       <c r="A150" s="46" t="s">
         <v>377</v>
       </c>
@@ -10472,7 +10472,7 @@
       </c>
       <c r="J150" s="95"/>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" ht="18.75">
       <c r="A151" s="31" t="s">
         <v>381</v>
       </c>
@@ -10502,7 +10502,7 @@
       </c>
       <c r="J151" s="95"/>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" ht="18.75">
       <c r="A152" s="46" t="s">
         <v>381</v>
       </c>
@@ -10532,7 +10532,7 @@
       </c>
       <c r="J152" s="35"/>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" ht="18.75">
       <c r="A153" s="31" t="s">
         <v>385</v>
       </c>
@@ -10562,7 +10562,7 @@
       </c>
       <c r="J153" s="95"/>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" ht="18.75">
       <c r="A154" s="31" t="s">
         <v>389</v>
       </c>
@@ -10592,7 +10592,7 @@
       </c>
       <c r="J154" s="95"/>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" ht="18.75">
       <c r="A155" s="31" t="s">
         <v>54</v>
       </c>
@@ -10622,7 +10622,7 @@
       </c>
       <c r="J155" s="104"/>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" ht="18.75">
       <c r="A156" s="28" t="s">
         <v>393</v>
       </c>
@@ -10652,7 +10652,7 @@
       </c>
       <c r="J156" s="53"/>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" ht="18.75">
       <c r="A157" s="182" t="s">
         <v>120</v>
       </c>
@@ -10682,7 +10682,7 @@
       </c>
       <c r="J157" s="187"/>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" ht="18.75">
       <c r="A158" s="182" t="s">
         <v>120</v>
       </c>
@@ -10712,7 +10712,7 @@
       </c>
       <c r="J158" s="187"/>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" ht="18.75">
       <c r="A159" s="28" t="s">
         <v>398</v>
       </c>
@@ -10742,7 +10742,7 @@
       </c>
       <c r="J159" s="36"/>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" ht="18.75">
       <c r="A160" s="31" t="s">
         <v>401</v>
       </c>
@@ -10772,7 +10772,7 @@
       </c>
       <c r="J160" s="53"/>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" ht="18.75">
       <c r="A161" s="46" t="s">
         <v>404</v>
       </c>
@@ -10802,7 +10802,7 @@
       </c>
       <c r="J161" s="67"/>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" ht="18.75">
       <c r="A162" s="31" t="s">
         <v>406</v>
       </c>
@@ -10832,7 +10832,7 @@
       </c>
       <c r="J162" s="53"/>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" ht="18.75">
       <c r="A163" s="182" t="s">
         <v>408</v>
       </c>
@@ -10862,7 +10862,7 @@
       </c>
       <c r="J163" s="187"/>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" ht="18.75">
       <c r="A164" s="182" t="s">
         <v>410</v>
       </c>
@@ -10892,7 +10892,7 @@
       </c>
       <c r="J164" s="53"/>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" ht="18.75">
       <c r="A165" s="46" t="s">
         <v>412</v>
       </c>
@@ -10922,7 +10922,7 @@
       </c>
       <c r="J165" s="67"/>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" ht="18.75">
       <c r="A166" s="46" t="s">
         <v>114</v>
       </c>
@@ -10952,7 +10952,7 @@
       </c>
       <c r="J166" s="67"/>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" ht="18.75">
       <c r="A167" s="46" t="s">
         <v>416</v>
       </c>
@@ -10982,7 +10982,7 @@
       </c>
       <c r="J167" s="53"/>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" ht="18.75">
       <c r="A168" s="46" t="s">
         <v>416</v>
       </c>
@@ -11012,7 +11012,7 @@
       </c>
       <c r="J168" s="53"/>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" ht="18.75">
       <c r="A169" s="46" t="s">
         <v>35</v>
       </c>
@@ -11042,7 +11042,7 @@
       </c>
       <c r="J169" s="53"/>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" ht="18.75">
       <c r="A170" s="46" t="s">
         <v>313</v>
       </c>
@@ -11072,7 +11072,7 @@
       </c>
       <c r="J170" s="53"/>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" ht="18.75">
       <c r="A171" s="28" t="s">
         <v>422</v>
       </c>
@@ -11102,7 +11102,7 @@
       </c>
       <c r="J171" s="53"/>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" ht="18.75">
       <c r="A172" s="28" t="s">
         <v>424</v>
       </c>
@@ -11132,7 +11132,7 @@
       </c>
       <c r="J172" s="53"/>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" ht="18.75">
       <c r="A173" s="28" t="s">
         <v>426</v>
       </c>
@@ -11162,7 +11162,7 @@
       </c>
       <c r="J173" s="53"/>
     </row>
-    <row r="174" spans="1:10" ht="20" customHeight="1">
+    <row r="174" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A174" s="28" t="s">
         <v>310</v>
       </c>
@@ -11192,7 +11192,7 @@
       </c>
       <c r="J174" s="53"/>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" ht="18.75">
       <c r="A175" s="46" t="s">
         <v>431</v>
       </c>
@@ -11222,7 +11222,7 @@
       </c>
       <c r="J175" s="67"/>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" ht="18.75">
       <c r="A176" s="28" t="s">
         <v>357</v>
       </c>
@@ -11252,7 +11252,7 @@
       </c>
       <c r="J176" s="35"/>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" ht="18.75">
       <c r="A177" s="28" t="s">
         <v>9</v>
       </c>
@@ -11282,7 +11282,7 @@
       </c>
       <c r="J177" s="53"/>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" ht="18.75">
       <c r="A178" s="118" t="s">
         <v>436</v>
       </c>
@@ -11312,7 +11312,7 @@
       </c>
       <c r="J178" s="121"/>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" ht="18.75">
       <c r="A179" s="194" t="s">
         <v>357</v>
       </c>
@@ -11342,7 +11342,7 @@
       </c>
       <c r="J179" s="201"/>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" ht="18.75">
       <c r="A180" s="28" t="s">
         <v>440</v>
       </c>
@@ -11372,7 +11372,7 @@
       </c>
       <c r="J180" s="53"/>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" ht="18.75">
       <c r="A181" s="28" t="s">
         <v>442</v>
       </c>
@@ -11402,7 +11402,7 @@
       </c>
       <c r="J181" s="53"/>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" ht="18.75">
       <c r="A182" s="28" t="s">
         <v>445</v>
       </c>
@@ -11432,7 +11432,7 @@
       </c>
       <c r="J182" s="53"/>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" ht="18.75">
       <c r="A183" s="28" t="s">
         <v>447</v>
       </c>
@@ -11462,7 +11462,7 @@
       </c>
       <c r="J183" s="53"/>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" ht="18.75">
       <c r="A184" s="28" t="s">
         <v>440</v>
       </c>
@@ -11492,7 +11492,7 @@
       </c>
       <c r="J184" s="53"/>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" ht="18.75">
       <c r="A185" s="28" t="s">
         <v>449</v>
       </c>
@@ -11522,7 +11522,7 @@
       </c>
       <c r="J185" s="53"/>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" ht="18.75">
       <c r="A186" s="28" t="s">
         <v>451</v>
       </c>
@@ -11552,7 +11552,7 @@
       </c>
       <c r="J186" s="53"/>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" ht="18.75">
       <c r="A187" s="28" t="s">
         <v>372</v>
       </c>
@@ -11578,7 +11578,7 @@
       <c r="I187" s="169"/>
       <c r="J187" s="53"/>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" ht="18.75">
       <c r="A188" s="28" t="s">
         <v>135</v>
       </c>
@@ -11608,7 +11608,7 @@
       </c>
       <c r="J188" s="53"/>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" ht="18.75">
       <c r="A189" s="28" t="s">
         <v>456</v>
       </c>
@@ -11638,7 +11638,7 @@
       </c>
       <c r="J189" s="53"/>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" ht="18.75">
       <c r="A190" s="28" t="s">
         <v>458</v>
       </c>
@@ -11668,7 +11668,7 @@
       </c>
       <c r="J190" s="53"/>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" ht="18.75">
       <c r="A191" s="204" t="s">
         <v>460</v>
       </c>
@@ -11698,7 +11698,7 @@
       </c>
       <c r="J191" s="210"/>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" ht="18.75">
       <c r="A192" s="46" t="s">
         <v>463</v>
       </c>
@@ -11728,7 +11728,7 @@
       </c>
       <c r="J192" s="67"/>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" ht="18.75">
       <c r="A193" s="28" t="s">
         <v>310</v>
       </c>
@@ -11758,7 +11758,7 @@
       </c>
       <c r="J193" s="53"/>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" ht="18.75">
       <c r="A194" s="28" t="s">
         <v>320</v>
       </c>
@@ -11788,7 +11788,7 @@
       </c>
       <c r="J194" s="53"/>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" ht="18.75">
       <c r="A195" s="130" t="s">
         <v>229</v>
       </c>
@@ -11818,7 +11818,7 @@
       </c>
       <c r="J195" s="135"/>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" ht="18.75">
       <c r="A196" s="21" t="s">
         <v>456</v>
       </c>
@@ -11848,7 +11848,7 @@
       </c>
       <c r="J196" s="8"/>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" ht="18.75">
       <c r="A197" s="21" t="s">
         <v>472</v>
       </c>
@@ -11878,7 +11878,7 @@
       </c>
       <c r="J197" s="8"/>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" ht="18.75">
       <c r="A198" s="136" t="s">
         <v>475</v>
       </c>
@@ -11904,7 +11904,7 @@
       </c>
       <c r="J198" s="142"/>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" ht="18.75">
       <c r="A199" s="28" t="s">
         <v>479</v>
       </c>
@@ -11934,7 +11934,7 @@
       </c>
       <c r="J199" s="53"/>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" ht="18.75">
       <c r="A200" s="28" t="s">
         <v>482</v>
       </c>
@@ -11964,7 +11964,7 @@
       </c>
       <c r="J200" s="53"/>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" ht="18.75">
       <c r="A201" s="28" t="s">
         <v>320</v>
       </c>
@@ -11994,7 +11994,7 @@
       </c>
       <c r="J201" s="53"/>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" ht="18.75">
       <c r="A202" s="28" t="s">
         <v>486</v>
       </c>
@@ -12024,7 +12024,7 @@
       </c>
       <c r="J202" s="53"/>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" ht="18.75">
       <c r="A203" s="217" t="s">
         <v>308</v>
       </c>
@@ -12054,7 +12054,7 @@
       </c>
       <c r="J203" s="224"/>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" ht="18.75">
       <c r="A204" s="217" t="s">
         <v>491</v>
       </c>
@@ -12084,7 +12084,7 @@
       </c>
       <c r="J204" s="227"/>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" ht="18.75">
       <c r="A205" s="28" t="s">
         <v>25</v>
       </c>
@@ -12114,7 +12114,7 @@
       </c>
       <c r="J205" s="36"/>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" ht="18.75">
       <c r="A206" s="217" t="s">
         <v>25</v>
       </c>
@@ -12144,7 +12144,7 @@
       </c>
       <c r="J206" s="227"/>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" ht="18.75">
       <c r="A207" s="28" t="s">
         <v>496</v>
       </c>
@@ -12174,7 +12174,7 @@
       </c>
       <c r="J207" s="36"/>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" ht="18.75">
       <c r="A208" s="28" t="s">
         <v>491</v>
       </c>
@@ -12204,7 +12204,7 @@
       </c>
       <c r="J208" s="36"/>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" ht="18.75">
       <c r="A209" s="28" t="s">
         <v>498</v>
       </c>
@@ -12234,7 +12234,7 @@
       </c>
       <c r="J209" s="36"/>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" ht="18.75">
       <c r="A210" s="217" t="s">
         <v>501</v>
       </c>
@@ -12264,7 +12264,7 @@
       </c>
       <c r="J210" s="224"/>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" ht="18.75">
       <c r="A211" s="28" t="s">
         <v>505</v>
       </c>
@@ -12292,7 +12292,7 @@
       </c>
       <c r="J211" s="53"/>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" ht="18.75">
       <c r="A212" s="28" t="s">
         <v>508</v>
       </c>
@@ -12322,7 +12322,7 @@
       </c>
       <c r="J212" s="53"/>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" ht="18.75">
       <c r="A213" s="28" t="s">
         <v>511</v>
       </c>
@@ -12352,7 +12352,7 @@
       </c>
       <c r="J213" s="53"/>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" ht="18.75">
       <c r="A214" s="28" t="s">
         <v>515</v>
       </c>
@@ -12382,7 +12382,7 @@
       </c>
       <c r="J214" s="53"/>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" ht="18.75">
       <c r="A215" s="28" t="s">
         <v>516</v>
       </c>
@@ -12412,7 +12412,7 @@
       </c>
       <c r="J215" s="53"/>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" ht="18.75">
       <c r="A216" s="217" t="s">
         <v>519</v>
       </c>
@@ -12442,7 +12442,7 @@
       </c>
       <c r="J216" s="224"/>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" ht="18.75">
       <c r="A217" s="28" t="s">
         <v>64</v>
       </c>
@@ -12472,7 +12472,7 @@
       </c>
       <c r="J217" s="53"/>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" ht="18.75">
       <c r="A218" s="28" t="s">
         <v>524</v>
       </c>
@@ -12502,7 +12502,7 @@
       </c>
       <c r="J218" s="36"/>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" ht="18.75">
       <c r="A219" s="217" t="s">
         <v>44</v>
       </c>
@@ -12532,7 +12532,7 @@
       </c>
       <c r="J219" s="224"/>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" ht="18.75">
       <c r="A220" s="217" t="s">
         <v>283</v>
       </c>
@@ -12562,7 +12562,7 @@
       </c>
       <c r="J220" s="224"/>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" ht="18.75">
       <c r="A221" s="217" t="s">
         <v>530</v>
       </c>
@@ -12592,7 +12592,7 @@
       </c>
       <c r="J221" s="224"/>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" ht="18.75">
       <c r="A222" s="217" t="s">
         <v>531</v>
       </c>
@@ -12622,7 +12622,7 @@
       </c>
       <c r="J222" s="224"/>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" ht="18.75">
       <c r="A223" s="217" t="s">
         <v>533</v>
       </c>
@@ -12652,7 +12652,7 @@
       </c>
       <c r="J223" s="224"/>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" ht="18.75">
       <c r="A224" s="28" t="s">
         <v>524</v>
       </c>
@@ -12682,7 +12682,7 @@
       </c>
       <c r="J224" s="36"/>
     </row>
-    <row r="225" spans="1:10" ht="20" customHeight="1">
+    <row r="225" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A225" s="28" t="s">
         <v>537</v>
       </c>
@@ -12712,7 +12712,7 @@
       </c>
       <c r="J225" s="53"/>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" ht="18.75">
       <c r="A226" s="28" t="s">
         <v>540</v>
       </c>
@@ -12742,7 +12742,7 @@
       </c>
       <c r="J226" s="53"/>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" ht="18.75">
       <c r="A227" s="28" t="s">
         <v>543</v>
       </c>
@@ -12772,7 +12772,7 @@
       </c>
       <c r="J227" s="53"/>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" ht="18.75">
       <c r="A228" s="217" t="s">
         <v>545</v>
       </c>
@@ -12802,7 +12802,7 @@
       </c>
       <c r="J228" s="224"/>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" ht="18.75">
       <c r="A229" s="28" t="s">
         <v>548</v>
       </c>
@@ -12832,7 +12832,7 @@
       </c>
       <c r="J229" s="53"/>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" ht="18.75">
       <c r="A230" s="28" t="s">
         <v>549</v>
       </c>
@@ -12862,7 +12862,7 @@
       </c>
       <c r="J230" s="36"/>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" ht="18.75">
       <c r="A231" s="217" t="s">
         <v>524</v>
       </c>
@@ -12892,7 +12892,7 @@
       </c>
       <c r="J231" s="227"/>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" ht="18.75">
       <c r="A232" s="28" t="s">
         <v>214</v>
       </c>
@@ -12922,7 +12922,7 @@
       </c>
       <c r="J232" s="53"/>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" ht="18.75">
       <c r="A233" s="28" t="s">
         <v>552</v>
       </c>
@@ -12952,7 +12952,7 @@
       </c>
       <c r="J233" s="53"/>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" ht="18.75">
       <c r="A234" s="28" t="s">
         <v>555</v>
       </c>
@@ -12982,7 +12982,7 @@
       </c>
       <c r="J234" s="53"/>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" ht="18.75">
       <c r="A235" s="28" t="s">
         <v>289</v>
       </c>
@@ -13012,7 +13012,7 @@
       </c>
       <c r="J235" s="53"/>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" ht="18.75">
       <c r="A236" s="28" t="s">
         <v>561</v>
       </c>
@@ -13042,7 +13042,7 @@
       </c>
       <c r="J236" s="53"/>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" ht="18.75">
       <c r="A237" s="28" t="s">
         <v>135</v>
       </c>
@@ -13072,7 +13072,7 @@
       </c>
       <c r="J237" s="53"/>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" ht="18.75">
       <c r="A238" s="28" t="s">
         <v>289</v>
       </c>
@@ -13102,7 +13102,7 @@
       </c>
       <c r="J238" s="53"/>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" ht="18.75">
       <c r="A239" s="28" t="s">
         <v>320</v>
       </c>
@@ -13132,7 +13132,7 @@
       </c>
       <c r="J239" s="53"/>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" ht="18.75">
       <c r="A240" s="28" t="s">
         <v>567</v>
       </c>
@@ -13162,7 +13162,7 @@
       </c>
       <c r="J240" s="53"/>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" ht="18.75">
       <c r="A241" s="28" t="s">
         <v>569</v>
       </c>
@@ -13192,7 +13192,7 @@
       </c>
       <c r="J241" s="53"/>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" ht="18.75">
       <c r="A242" s="46" t="s">
         <v>573</v>
       </c>
@@ -13222,7 +13222,7 @@
       </c>
       <c r="J242" s="67"/>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" ht="18.75">
       <c r="A243" s="28" t="s">
         <v>577</v>
       </c>
@@ -13252,7 +13252,7 @@
       </c>
       <c r="J243" s="53"/>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" ht="18.75">
       <c r="A244" s="28" t="s">
         <v>120</v>
       </c>
@@ -13282,7 +13282,7 @@
       </c>
       <c r="J244" s="53"/>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" ht="18.75">
       <c r="A245" s="28" t="s">
         <v>530</v>
       </c>
@@ -13312,7 +13312,7 @@
       </c>
       <c r="J245" s="53"/>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" ht="18.75">
       <c r="A246" s="28" t="s">
         <v>320</v>
       </c>
@@ -13342,7 +13342,7 @@
       </c>
       <c r="J246" s="53"/>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" ht="18.75">
       <c r="A247" s="28" t="s">
         <v>586</v>
       </c>
@@ -13372,7 +13372,7 @@
       </c>
       <c r="J247" s="53"/>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" ht="18.75">
       <c r="A248" s="28" t="s">
         <v>289</v>
       </c>
@@ -13402,7 +13402,7 @@
       </c>
       <c r="J248" s="53"/>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" ht="18.75">
       <c r="A249" s="28" t="s">
         <v>590</v>
       </c>
@@ -13432,7 +13432,7 @@
       </c>
       <c r="J249" s="67"/>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" ht="18.75">
       <c r="A250" s="239" t="s">
         <v>592</v>
       </c>
@@ -13462,7 +13462,7 @@
       </c>
       <c r="J250" s="246"/>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" ht="18.75">
       <c r="A251" s="217" t="s">
         <v>593</v>
       </c>
@@ -13492,7 +13492,7 @@
       </c>
       <c r="J251" s="224"/>
     </row>
-    <row r="252" spans="1:10">
+    <row r="252" spans="1:10" ht="18.75">
       <c r="A252" s="28" t="s">
         <v>596</v>
       </c>
@@ -13522,7 +13522,7 @@
       </c>
       <c r="J252" s="53"/>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" ht="18.75">
       <c r="A253" s="28" t="s">
         <v>440</v>
       </c>
@@ -13552,7 +13552,7 @@
       </c>
       <c r="J253" s="67"/>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" ht="18.75">
       <c r="A254" s="28" t="s">
         <v>39</v>
       </c>
@@ -13582,7 +13582,7 @@
       </c>
       <c r="J254" s="67"/>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:10" ht="18.75">
       <c r="A255" s="28" t="s">
         <v>602</v>
       </c>
@@ -13612,7 +13612,7 @@
       </c>
       <c r="J255" s="67"/>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" ht="18.75">
       <c r="A256" s="28" t="s">
         <v>604</v>
       </c>
@@ -13642,7 +13642,7 @@
       </c>
       <c r="J256" s="67"/>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:10" ht="18.75">
       <c r="A257" s="28" t="s">
         <v>606</v>
       </c>
@@ -13672,7 +13672,7 @@
       </c>
       <c r="J257" s="67"/>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" ht="18.75">
       <c r="A258" s="28" t="s">
         <v>608</v>
       </c>
@@ -13702,7 +13702,7 @@
       </c>
       <c r="J258" s="67"/>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" ht="18.75">
       <c r="A259" s="28" t="s">
         <v>586</v>
       </c>
@@ -13732,7 +13732,7 @@
       </c>
       <c r="J259" s="67"/>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" ht="18.75">
       <c r="A260" s="28" t="s">
         <v>608</v>
       </c>
@@ -13759,7 +13759,7 @@
       </c>
       <c r="J260" s="67"/>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" ht="18.75">
       <c r="A261" s="28" t="s">
         <v>612</v>
       </c>
@@ -13789,7 +13789,7 @@
       </c>
       <c r="J261" s="67"/>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:10" ht="18.75">
       <c r="A262" s="46" t="s">
         <v>614</v>
       </c>
@@ -13819,7 +13819,7 @@
       </c>
       <c r="J262" s="67"/>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:10" ht="18.75">
       <c r="A263" s="46" t="s">
         <v>614</v>
       </c>
@@ -13849,7 +13849,7 @@
       </c>
       <c r="J263" s="67"/>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:10" ht="18.75">
       <c r="A264" s="46" t="s">
         <v>619</v>
       </c>
@@ -13879,7 +13879,7 @@
       </c>
       <c r="J264" s="35"/>
     </row>
-    <row r="265" spans="1:10" customFormat="1">
+    <row r="265" spans="1:10" customFormat="1" ht="18.75">
       <c r="A265" s="28" t="s">
         <v>177</v>
       </c>
@@ -13907,7 +13907,7 @@
       </c>
       <c r="J265" s="67"/>
     </row>
-    <row r="266" spans="1:10">
+    <row r="266" spans="1:10" ht="18.75">
       <c r="A266" s="28" t="s">
         <v>177</v>
       </c>
@@ -13930,7 +13930,7 @@
       </c>
       <c r="J266" s="67"/>
     </row>
-    <row r="267" spans="1:10">
+    <row r="267" spans="1:10" ht="18.75">
       <c r="A267" s="28" t="s">
         <v>236</v>
       </c>
@@ -13958,7 +13958,7 @@
       </c>
       <c r="J267" s="67"/>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:10" ht="18.75">
       <c r="A268" s="28" t="s">
         <v>625</v>
       </c>
@@ -13984,7 +13984,7 @@
       </c>
       <c r="J268" s="67"/>
     </row>
-    <row r="269" spans="1:10">
+    <row r="269" spans="1:10" ht="18.75">
       <c r="A269" s="217" t="s">
         <v>236</v>
       </c>
@@ -14008,7 +14008,7 @@
       <c r="I269" s="252"/>
       <c r="J269" s="253"/>
     </row>
-    <row r="270" spans="1:10">
+    <row r="270" spans="1:10" ht="18.75">
       <c r="A270" s="86" t="s">
         <v>628</v>
       </c>
@@ -14032,7 +14032,7 @@
       </c>
       <c r="J270" s="155"/>
     </row>
-    <row r="271" spans="1:10">
+    <row r="271" spans="1:10" ht="18.75">
       <c r="A271" s="86" t="s">
         <v>632</v>
       </c>
@@ -14056,7 +14056,7 @@
       </c>
       <c r="J271" s="155"/>
     </row>
-    <row r="272" spans="1:10">
+    <row r="272" spans="1:10" ht="18.75">
       <c r="A272" s="86" t="s">
         <v>44</v>
       </c>
@@ -14080,7 +14080,7 @@
       </c>
       <c r="J272" s="35"/>
     </row>
-    <row r="273" spans="1:10">
+    <row r="273" spans="1:10" ht="18.75">
       <c r="A273" s="86" t="s">
         <v>44</v>
       </c>
@@ -14104,7 +14104,7 @@
       </c>
       <c r="J273" s="35"/>
     </row>
-    <row r="274" spans="1:10">
+    <row r="274" spans="1:10" ht="18.75">
       <c r="A274" s="86" t="s">
         <v>637</v>
       </c>
@@ -14128,7 +14128,7 @@
       </c>
       <c r="J274" s="37"/>
     </row>
-    <row r="275" spans="1:10">
+    <row r="275" spans="1:10" ht="18.75">
       <c r="A275" s="86" t="s">
         <v>639</v>
       </c>
@@ -14152,7 +14152,7 @@
       </c>
       <c r="J275" s="37"/>
     </row>
-    <row r="276" spans="1:10">
+    <row r="276" spans="1:10" ht="18.75">
       <c r="A276" s="86" t="s">
         <v>642</v>
       </c>
@@ -14176,7 +14176,7 @@
       </c>
       <c r="J276" s="37"/>
     </row>
-    <row r="277" spans="1:10">
+    <row r="277" spans="1:10" ht="18.75">
       <c r="A277" s="86"/>
       <c r="B277" s="87"/>
       <c r="C277" s="86" t="s">
@@ -14194,7 +14194,7 @@
       <c r="I277" s="257"/>
       <c r="J277" s="37"/>
     </row>
-    <row r="278" spans="1:10">
+    <row r="278" spans="1:10" ht="18.75">
       <c r="A278" s="86" t="s">
         <v>68</v>
       </c>
@@ -14218,7 +14218,7 @@
       </c>
       <c r="J278" s="37"/>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:10" ht="18.75">
       <c r="A279" s="86" t="s">
         <v>646</v>
       </c>
@@ -14242,7 +14242,7 @@
       </c>
       <c r="J279" s="35"/>
     </row>
-    <row r="280" spans="1:10">
+    <row r="280" spans="1:10" ht="18.75">
       <c r="A280" s="86" t="s">
         <v>647</v>
       </c>
@@ -14266,7 +14266,7 @@
       </c>
       <c r="J280" s="37"/>
     </row>
-    <row r="281" spans="1:10">
+    <row r="281" spans="1:10" ht="18.75">
       <c r="A281" s="86" t="s">
         <v>648</v>
       </c>
@@ -14290,7 +14290,7 @@
       </c>
       <c r="J281" s="37"/>
     </row>
-    <row r="282" spans="1:10">
+    <row r="282" spans="1:10" ht="18.75">
       <c r="A282" s="86" t="s">
         <v>651</v>
       </c>
@@ -14312,7 +14312,7 @@
       </c>
       <c r="J282" s="37"/>
     </row>
-    <row r="283" spans="1:10">
+    <row r="283" spans="1:10" ht="18.75">
       <c r="A283" s="130"/>
       <c r="B283" s="125"/>
       <c r="C283" s="130"/>
@@ -14327,7 +14327,7 @@
       <c r="I283" s="146"/>
       <c r="J283" s="146"/>
     </row>
-    <row r="284" spans="1:10" customFormat="1">
+    <row r="284" spans="1:10" customFormat="1" ht="18.75">
       <c r="A284" s="86"/>
       <c r="B284" s="87"/>
       <c r="C284" s="86"/>
@@ -14339,7 +14339,7 @@
       <c r="I284" s="93"/>
       <c r="J284" s="35"/>
     </row>
-    <row r="285" spans="1:10">
+    <row r="285" spans="1:10" ht="18.75">
       <c r="A285" s="86"/>
       <c r="B285" s="87"/>
       <c r="C285" s="86"/>
@@ -14351,7 +14351,7 @@
       <c r="I285" s="37"/>
       <c r="J285" s="37"/>
     </row>
-    <row r="286" spans="1:10">
+    <row r="286" spans="1:10" ht="18.75">
       <c r="A286" s="86"/>
       <c r="B286" s="87"/>
       <c r="C286" s="86"/>
@@ -14363,7 +14363,7 @@
       <c r="I286" s="37"/>
       <c r="J286" s="37"/>
     </row>
-    <row r="287" spans="1:10">
+    <row r="287" spans="1:10" ht="18.75">
       <c r="A287" s="86"/>
       <c r="B287" s="87"/>
       <c r="C287" s="86"/>
@@ -14375,7 +14375,7 @@
       <c r="I287" s="37"/>
       <c r="J287" s="37"/>
     </row>
-    <row r="288" spans="1:10">
+    <row r="288" spans="1:10" ht="18.75">
       <c r="A288" s="28"/>
       <c r="B288" s="4"/>
       <c r="C288" s="28"/>
@@ -14387,7 +14387,7 @@
       <c r="I288" s="36"/>
       <c r="J288" s="36"/>
     </row>
-    <row r="289" spans="1:10">
+    <row r="289" spans="1:10" ht="18.75">
       <c r="A289" s="21"/>
       <c r="B289" s="19"/>
       <c r="C289" s="22"/>
@@ -14417,18 +14417,18 @@
       <selection activeCell="A2" sqref="A2 A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="9.1796875" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" customHeight="1">

</xml_diff>